<commit_message>
Updated Files for Systemtest #65 #62
</commit_message>
<xml_diff>
--- a/Basisverzeichnis/trunk/04_Test/Systemtest_TestCases.xlsx
+++ b/Basisverzeichnis/trunk/04_Test/Systemtest_TestCases.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="160">
   <si>
     <t>Nr.</t>
   </si>
@@ -287,11 +287,6 @@
   <si>
     <t>Test-Datei: UseCase_Correct_Abstract.docx
 liegt vor und ist vom Tool eingelesen</t>
-  </si>
-  <si>
-    <t>1. Der Anwender wählt jeden einzelnen UseCase aus, lässt ihn darstellen und vergleicht ihn mit der Darstellung in der Datei
-UseCase_Abstract_Darstellungen.docx
-2. Test erfolgreich wenn Darstellungen identisch sind</t>
   </si>
   <si>
     <t>Zweiter Testdurchlauf Auswertung</t>
@@ -623,6 +618,20 @@
 sind vorhanden
 </t>
   </si>
+  <si>
+    <t>1. Der Anwender wählt jeden einzelnen UseCase aus, lässt ihn darstellen und vergleicht ihn mit der Darstellung in der Datei
+Darstellungen_UseCase_Abstract.docx
+2. Test erfolgreich wenn Darstellungen identisch sind</t>
+  </si>
+  <si>
+    <t>Mit Beyond Compare am 29.06.15 getestet</t>
+  </si>
+  <si>
+    <t>Anpassungen der Darstellungen waren notwendig aufgrund Funktionalitätsänderung (Ende - Knoten entfernt)</t>
+  </si>
+  <si>
+    <t>Dritter Testdurchlauf am 29.06.2015</t>
+  </si>
 </sst>
 </file>
 
@@ -934,7 +943,7 @@
     <xf numFmtId="0" fontId="5" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1131,6 +1140,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1146,20 +1158,20 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1167,8 +1179,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -5653,8 +5665,8 @@
   </sheetPr>
   <dimension ref="A1:T199"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5671,7 +5683,7 @@
     <col min="10" max="10" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="23" customWidth="1"/>
     <col min="12" max="12" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.7109375" customWidth="1"/>
+    <col min="13" max="13" width="29.140625" customWidth="1"/>
     <col min="14" max="14" width="18.28515625" customWidth="1"/>
     <col min="15" max="15" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="24.42578125" customWidth="1"/>
@@ -5689,15 +5701,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="85" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
       <c r="H1" s="12"/>
       <c r="I1" s="7"/>
       <c r="J1" s="12"/>
@@ -5711,15 +5723,15 @@
       <c r="R1" s="7"/>
     </row>
     <row r="2" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="81"/>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
       <c r="H2" s="12"/>
       <c r="I2" s="7"/>
       <c r="J2" s="12"/>
@@ -5750,7 +5762,7 @@
       <c r="D4" s="19"/>
       <c r="E4" s="22"/>
       <c r="F4" s="22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -5764,7 +5776,7 @@
       <c r="D5" s="19"/>
       <c r="E5" s="22"/>
       <c r="F5" s="22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H5"/>
       <c r="J5"/>
@@ -5780,7 +5792,9 @@
       </c>
       <c r="D6" s="19"/>
       <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
+      <c r="F6" s="22" t="s">
+        <v>159</v>
+      </c>
       <c r="H6"/>
       <c r="J6"/>
       <c r="L6"/>
@@ -5803,7 +5817,7 @@
       </c>
       <c r="D8" s="19"/>
       <c r="E8" s="22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F8" s="22"/>
     </row>
@@ -5814,27 +5828,27 @@
       <c r="F9" s="22"/>
     </row>
     <row r="10" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="73" t="s">
+      <c r="A10" s="74" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="73"/>
-      <c r="C10" s="73"/>
-      <c r="D10" s="73"/>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="74"/>
-      <c r="H10" s="75" t="s">
+      <c r="B10" s="74"/>
+      <c r="C10" s="74"/>
+      <c r="D10" s="74"/>
+      <c r="E10" s="74"/>
+      <c r="F10" s="74"/>
+      <c r="G10" s="75"/>
+      <c r="H10" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="I10" s="76"/>
-      <c r="J10" s="75" t="s">
+      <c r="I10" s="77"/>
+      <c r="J10" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="K10" s="76"/>
-      <c r="L10" s="75" t="s">
+      <c r="K10" s="77"/>
+      <c r="L10" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="M10" s="76"/>
+      <c r="M10" s="77"/>
       <c r="O10"/>
       <c r="Q10"/>
     </row>
@@ -5842,10 +5856,10 @@
       <c r="A11" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="82" t="s">
+      <c r="B11" s="83" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="82"/>
+      <c r="C11" s="83"/>
       <c r="D11" s="9" t="s">
         <v>1</v>
       </c>
@@ -5883,12 +5897,12 @@
       <c r="A12" s="30">
         <v>1</v>
       </c>
-      <c r="B12" s="83" t="s">
+      <c r="B12" s="84" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="83"/>
+      <c r="C12" s="84"/>
       <c r="D12" s="34" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E12" s="32" t="s">
         <v>31</v>
@@ -5910,7 +5924,7 @@
       </c>
       <c r="K12" s="33"/>
       <c r="L12" s="31" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="M12" s="33"/>
       <c r="O12"/>
@@ -5920,12 +5934,12 @@
       <c r="A13" s="35">
         <v>2</v>
       </c>
-      <c r="B13" s="69" t="s">
+      <c r="B13" s="78" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="69"/>
+      <c r="C13" s="78"/>
       <c r="D13" s="34" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E13" s="32" t="s">
         <v>37</v>
@@ -5945,7 +5959,7 @@
       </c>
       <c r="K13" s="33"/>
       <c r="L13" s="31" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="M13" s="33"/>
       <c r="O13"/>
@@ -5955,12 +5969,12 @@
       <c r="A14" s="30">
         <v>3</v>
       </c>
-      <c r="B14" s="69" t="s">
+      <c r="B14" s="78" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="69"/>
+      <c r="C14" s="78"/>
       <c r="D14" s="34" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E14" s="32" t="s">
         <v>38</v>
@@ -5980,7 +5994,7 @@
       </c>
       <c r="K14" s="33"/>
       <c r="L14" s="31" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="M14" s="33"/>
       <c r="O14"/>
@@ -5997,22 +6011,22 @@
       <c r="B16" s="70"/>
       <c r="C16" s="70"/>
       <c r="F16" s="13"/>
-      <c r="H16" s="72" t="s">
+      <c r="H16" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="I16" s="72"/>
-      <c r="J16" s="72"/>
-      <c r="K16" s="72"/>
-      <c r="L16" s="72"/>
-      <c r="M16" s="72"/>
-      <c r="O16" s="72" t="s">
-        <v>83</v>
-      </c>
-      <c r="P16" s="72"/>
-      <c r="Q16" s="72"/>
-      <c r="R16" s="72"/>
-      <c r="S16" s="72"/>
-      <c r="T16" s="72"/>
+      <c r="I16" s="73"/>
+      <c r="J16" s="73"/>
+      <c r="K16" s="73"/>
+      <c r="L16" s="73"/>
+      <c r="M16" s="73"/>
+      <c r="O16" s="73" t="s">
+        <v>82</v>
+      </c>
+      <c r="P16" s="73"/>
+      <c r="Q16" s="73"/>
+      <c r="R16" s="73"/>
+      <c r="S16" s="73"/>
+      <c r="T16" s="73"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B17" s="70"/>
@@ -6127,14 +6141,14 @@
       <c r="K20" s="71"/>
       <c r="L20" s="71"/>
       <c r="M20" s="71"/>
-      <c r="O20" s="72" t="s">
-        <v>84</v>
-      </c>
-      <c r="P20" s="72"/>
-      <c r="Q20" s="72"/>
-      <c r="R20" s="72"/>
-      <c r="S20" s="72"/>
-      <c r="T20" s="72"/>
+      <c r="O20" s="73" t="s">
+        <v>83</v>
+      </c>
+      <c r="P20" s="73"/>
+      <c r="Q20" s="73"/>
+      <c r="R20" s="73"/>
+      <c r="S20" s="73"/>
+      <c r="T20" s="73"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B21" s="70"/>
@@ -6183,7 +6197,7 @@
       <c r="F22" s="13"/>
       <c r="H22" s="14">
         <f>H18+O18+O22</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I22" s="14">
         <f>I18+P18+P22</f>
@@ -6195,7 +6209,7 @@
       </c>
       <c r="K22" s="14">
         <f>K18+R18+R22</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="L22" s="14">
         <f>SUM(H22:K22)</f>
@@ -6203,11 +6217,11 @@
       </c>
       <c r="M22" s="15">
         <f>(K22+I22)/L22</f>
-        <v>0.55555555555555558</v>
+        <v>0.88888888888888884</v>
       </c>
       <c r="O22" s="14">
         <f>COUNTIF(L12:L14,"O")</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P22" s="14">
         <f>COUNTIF(J16:J18,"N")</f>
@@ -6219,7 +6233,7 @@
       </c>
       <c r="R22" s="14">
         <f>COUNTIF(L12:L14,"R")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S22" s="14">
         <f>SUM(O22:R22)</f>
@@ -6227,7 +6241,7 @@
       </c>
       <c r="T22" s="15">
         <f>(R22+P22)/S22</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6248,27 +6262,27 @@
       <c r="Q24"/>
     </row>
     <row r="25" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="73" t="s">
+      <c r="A25" s="74" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="73"/>
-      <c r="C25" s="73"/>
-      <c r="D25" s="73"/>
-      <c r="E25" s="73"/>
-      <c r="F25" s="73"/>
-      <c r="G25" s="74"/>
-      <c r="H25" s="75" t="s">
+      <c r="B25" s="74"/>
+      <c r="C25" s="74"/>
+      <c r="D25" s="74"/>
+      <c r="E25" s="74"/>
+      <c r="F25" s="74"/>
+      <c r="G25" s="75"/>
+      <c r="H25" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="I25" s="76"/>
-      <c r="J25" s="75" t="s">
+      <c r="I25" s="77"/>
+      <c r="J25" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="K25" s="76"/>
-      <c r="L25" s="75" t="s">
+      <c r="K25" s="77"/>
+      <c r="L25" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="M25" s="76"/>
+      <c r="M25" s="77"/>
       <c r="O25" s="23"/>
       <c r="Q25" s="23"/>
     </row>
@@ -6276,10 +6290,10 @@
       <c r="A26" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="77" t="s">
+      <c r="B26" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="77"/>
+      <c r="C26" s="79"/>
       <c r="D26" s="17" t="s">
         <v>1</v>
       </c>
@@ -6317,18 +6331,18 @@
       <c r="A27" s="30">
         <v>4</v>
       </c>
-      <c r="B27" s="78" t="s">
+      <c r="B27" s="80" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="78"/>
+      <c r="C27" s="80"/>
       <c r="D27" s="34" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E27" s="32" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F27" s="29" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G27" s="30" t="s">
         <v>32</v>
@@ -6337,16 +6351,16 @@
         <v>10</v>
       </c>
       <c r="I27" s="44" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J27" s="31" t="s">
         <v>12</v>
       </c>
       <c r="K27" s="54" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L27" s="31" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="M27" s="31"/>
       <c r="O27" s="23"/>
@@ -6356,18 +6370,18 @@
       <c r="A28" s="30">
         <v>5</v>
       </c>
-      <c r="B28" s="80" t="s">
+      <c r="B28" s="81" t="s">
         <v>30</v>
       </c>
-      <c r="C28" s="80"/>
+      <c r="C28" s="81"/>
       <c r="D28" s="34" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E28" s="32" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F28" s="29" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G28" s="30" t="s">
         <v>32</v>
@@ -6376,16 +6390,16 @@
         <v>10</v>
       </c>
       <c r="I28" s="44" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J28" s="31" t="s">
         <v>10</v>
       </c>
       <c r="K28" s="54" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L28" s="31" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="M28" s="31"/>
       <c r="O28" s="23"/>
@@ -6395,18 +6409,18 @@
       <c r="A29" s="58">
         <v>6</v>
       </c>
-      <c r="B29" s="78" t="s">
+      <c r="B29" s="80" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="78"/>
+      <c r="C29" s="80"/>
       <c r="D29" s="34" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E29" s="32" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F29" s="29" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G29" s="58" t="s">
         <v>32</v>
@@ -6420,7 +6434,7 @@
       </c>
       <c r="K29" s="58"/>
       <c r="L29" s="31" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="M29" s="31"/>
       <c r="O29" s="56"/>
@@ -6430,18 +6444,18 @@
       <c r="A30" s="58">
         <v>7</v>
       </c>
-      <c r="B30" s="80" t="s">
+      <c r="B30" s="81" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="80"/>
+      <c r="C30" s="81"/>
       <c r="D30" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="E30" s="32" t="s">
+        <v>139</v>
+      </c>
+      <c r="F30" s="29" t="s">
         <v>142</v>
-      </c>
-      <c r="E30" s="32" t="s">
-        <v>140</v>
-      </c>
-      <c r="F30" s="29" t="s">
-        <v>143</v>
       </c>
       <c r="G30" s="58" t="s">
         <v>32</v>
@@ -6455,7 +6469,7 @@
       </c>
       <c r="K30" s="58"/>
       <c r="L30" s="31" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="M30" s="31"/>
       <c r="O30" s="56"/>
@@ -6463,8 +6477,8 @@
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="27"/>
-      <c r="B31" s="84"/>
-      <c r="C31" s="84"/>
+      <c r="B31" s="82"/>
+      <c r="C31" s="82"/>
       <c r="D31" s="28"/>
       <c r="E31" s="29"/>
       <c r="F31" s="29"/>
@@ -6492,22 +6506,22 @@
       <c r="B33" s="70"/>
       <c r="C33" s="70"/>
       <c r="F33" s="13"/>
-      <c r="H33" s="72" t="s">
+      <c r="H33" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="I33" s="72"/>
-      <c r="J33" s="72"/>
-      <c r="K33" s="72"/>
-      <c r="L33" s="72"/>
-      <c r="M33" s="72"/>
-      <c r="O33" s="72" t="s">
-        <v>83</v>
-      </c>
-      <c r="P33" s="72"/>
-      <c r="Q33" s="72"/>
-      <c r="R33" s="72"/>
-      <c r="S33" s="72"/>
-      <c r="T33" s="72"/>
+      <c r="I33" s="73"/>
+      <c r="J33" s="73"/>
+      <c r="K33" s="73"/>
+      <c r="L33" s="73"/>
+      <c r="M33" s="73"/>
+      <c r="O33" s="73" t="s">
+        <v>82</v>
+      </c>
+      <c r="P33" s="73"/>
+      <c r="Q33" s="73"/>
+      <c r="R33" s="73"/>
+      <c r="S33" s="73"/>
+      <c r="T33" s="73"/>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B34" s="70"/>
@@ -6625,14 +6639,14 @@
       <c r="K37" s="71"/>
       <c r="L37" s="71"/>
       <c r="M37" s="71"/>
-      <c r="O37" s="72" t="s">
-        <v>84</v>
-      </c>
-      <c r="P37" s="72"/>
-      <c r="Q37" s="72"/>
-      <c r="R37" s="72"/>
-      <c r="S37" s="72"/>
-      <c r="T37" s="72"/>
+      <c r="O37" s="73" t="s">
+        <v>83</v>
+      </c>
+      <c r="P37" s="73"/>
+      <c r="Q37" s="73"/>
+      <c r="R37" s="73"/>
+      <c r="S37" s="73"/>
+      <c r="T37" s="73"/>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B38" s="70"/>
@@ -6681,7 +6695,7 @@
       <c r="F39" s="13"/>
       <c r="H39" s="14">
         <f>H35+O35+O39</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I39" s="14">
         <f>I35+P35+P39</f>
@@ -6693,7 +6707,7 @@
       </c>
       <c r="K39" s="14">
         <f>K35+R35+R39</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="L39" s="14">
         <f>SUM(H39:K39)</f>
@@ -6701,11 +6715,11 @@
       </c>
       <c r="M39" s="15">
         <f>(K39+I39)/L39</f>
-        <v>0.41666666666666669</v>
+        <v>0.75</v>
       </c>
       <c r="O39" s="14">
         <f>COUNTIF(L27:L31,"O")</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="P39" s="14">
         <f>COUNTIF(J33:J35,"N")</f>
@@ -6717,7 +6731,7 @@
       </c>
       <c r="R39" s="14">
         <f>COUNTIF(L27:L31,"R")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S39" s="14">
         <f>SUM(O39:R39)</f>
@@ -6725,7 +6739,7 @@
       </c>
       <c r="T39" s="15">
         <f>(R39+P39)/S39</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
@@ -6739,36 +6753,36 @@
       <c r="Q40" s="23"/>
     </row>
     <row r="41" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A41" s="73" t="s">
+      <c r="A41" s="74" t="s">
         <v>41</v>
       </c>
-      <c r="B41" s="73"/>
-      <c r="C41" s="73"/>
-      <c r="D41" s="73"/>
-      <c r="E41" s="73"/>
-      <c r="F41" s="73"/>
-      <c r="G41" s="74"/>
-      <c r="H41" s="75" t="s">
+      <c r="B41" s="74"/>
+      <c r="C41" s="74"/>
+      <c r="D41" s="74"/>
+      <c r="E41" s="74"/>
+      <c r="F41" s="74"/>
+      <c r="G41" s="75"/>
+      <c r="H41" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="I41" s="76"/>
-      <c r="J41" s="75" t="s">
+      <c r="I41" s="77"/>
+      <c r="J41" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="K41" s="76"/>
-      <c r="L41" s="75" t="s">
+      <c r="K41" s="77"/>
+      <c r="L41" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="M41" s="76"/>
+      <c r="M41" s="77"/>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B42" s="77" t="s">
+      <c r="B42" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="C42" s="77"/>
+      <c r="C42" s="79"/>
       <c r="D42" s="26" t="s">
         <v>1</v>
       </c>
@@ -6804,12 +6818,12 @@
       <c r="A43" s="35">
         <v>8</v>
       </c>
-      <c r="B43" s="78" t="s">
+      <c r="B43" s="80" t="s">
         <v>30</v>
       </c>
-      <c r="C43" s="78"/>
+      <c r="C43" s="80"/>
       <c r="D43" s="34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E43" s="32" t="s">
         <v>42</v>
@@ -6824,14 +6838,14 @@
         <v>12</v>
       </c>
       <c r="I43" s="44" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J43" s="31" t="s">
         <v>12</v>
       </c>
       <c r="K43" s="31"/>
       <c r="L43" s="31" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="M43" s="31"/>
     </row>
@@ -6839,18 +6853,18 @@
       <c r="A44" s="35">
         <v>9</v>
       </c>
-      <c r="B44" s="80" t="s">
+      <c r="B44" s="81" t="s">
         <v>30</v>
       </c>
-      <c r="C44" s="80"/>
+      <c r="C44" s="81"/>
       <c r="D44" s="34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E44" s="32" t="s">
         <v>43</v>
       </c>
       <c r="F44" s="29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G44" s="35" t="s">
         <v>32</v>
@@ -6864,7 +6878,7 @@
       </c>
       <c r="K44" s="31"/>
       <c r="L44" s="31" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="M44" s="31"/>
     </row>
@@ -6872,10 +6886,10 @@
       <c r="A45" s="35">
         <v>10</v>
       </c>
-      <c r="B45" s="69" t="s">
+      <c r="B45" s="78" t="s">
         <v>30</v>
       </c>
-      <c r="C45" s="69"/>
+      <c r="C45" s="78"/>
       <c r="D45" s="34" t="s">
         <v>45</v>
       </c>
@@ -6897,7 +6911,7 @@
       </c>
       <c r="K45" s="31"/>
       <c r="L45" s="31" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="M45" s="31"/>
     </row>
@@ -6905,18 +6919,18 @@
       <c r="A46" s="68">
         <v>11</v>
       </c>
-      <c r="B46" s="69" t="s">
+      <c r="B46" s="78" t="s">
         <v>30</v>
       </c>
-      <c r="C46" s="69"/>
+      <c r="C46" s="78"/>
       <c r="D46" s="34" t="s">
+        <v>150</v>
+      </c>
+      <c r="E46" s="32" t="s">
+        <v>149</v>
+      </c>
+      <c r="F46" s="29" t="s">
         <v>151</v>
-      </c>
-      <c r="E46" s="32" t="s">
-        <v>150</v>
-      </c>
-      <c r="F46" s="29" t="s">
-        <v>152</v>
       </c>
       <c r="G46" s="68" t="s">
         <v>32</v>
@@ -6930,7 +6944,7 @@
       </c>
       <c r="K46" s="31"/>
       <c r="L46" s="31" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="M46" s="31"/>
       <c r="O46" s="67"/>
@@ -6948,22 +6962,22 @@
       <c r="B48" s="70"/>
       <c r="C48" s="70"/>
       <c r="F48" s="13"/>
-      <c r="H48" s="72" t="s">
+      <c r="H48" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="I48" s="72"/>
-      <c r="J48" s="72"/>
-      <c r="K48" s="72"/>
-      <c r="L48" s="72"/>
-      <c r="M48" s="72"/>
-      <c r="O48" s="72" t="s">
-        <v>83</v>
-      </c>
-      <c r="P48" s="72"/>
-      <c r="Q48" s="72"/>
-      <c r="R48" s="72"/>
-      <c r="S48" s="72"/>
-      <c r="T48" s="72"/>
+      <c r="I48" s="73"/>
+      <c r="J48" s="73"/>
+      <c r="K48" s="73"/>
+      <c r="L48" s="73"/>
+      <c r="M48" s="73"/>
+      <c r="O48" s="73" t="s">
+        <v>82</v>
+      </c>
+      <c r="P48" s="73"/>
+      <c r="Q48" s="73"/>
+      <c r="R48" s="73"/>
+      <c r="S48" s="73"/>
+      <c r="T48" s="73"/>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B49" s="70"/>
@@ -7081,14 +7095,14 @@
       <c r="K52" s="71"/>
       <c r="L52" s="71"/>
       <c r="M52" s="71"/>
-      <c r="O52" s="72" t="s">
-        <v>84</v>
-      </c>
-      <c r="P52" s="72"/>
-      <c r="Q52" s="72"/>
-      <c r="R52" s="72"/>
-      <c r="S52" s="72"/>
-      <c r="T52" s="72"/>
+      <c r="O52" s="73" t="s">
+        <v>83</v>
+      </c>
+      <c r="P52" s="73"/>
+      <c r="Q52" s="73"/>
+      <c r="R52" s="73"/>
+      <c r="S52" s="73"/>
+      <c r="T52" s="73"/>
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B53" s="70"/>
@@ -7137,7 +7151,7 @@
       <c r="F54" s="13"/>
       <c r="H54" s="14">
         <f>H50+O50+O54</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I54" s="14">
         <f>I50+P50+P54</f>
@@ -7149,7 +7163,7 @@
       </c>
       <c r="K54" s="14">
         <f>K50+R50+R54</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="L54" s="14">
         <f>SUM(H54:K54)</f>
@@ -7157,11 +7171,11 @@
       </c>
       <c r="M54" s="15">
         <f>(K54+I54)/L54</f>
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
       <c r="O54" s="14">
         <f>COUNTIF(L43:L45,"O")</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P54" s="14">
         <f>COUNTIF(J48:J50,"N")</f>
@@ -7173,7 +7187,7 @@
       </c>
       <c r="R54" s="14">
         <f>COUNTIF(L43:L45,"R")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S54" s="14">
         <f>SUM(O54:R54)</f>
@@ -7181,12 +7195,12 @@
       </c>
       <c r="T54" s="15">
         <f>(R54+P54)/S54</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:20" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="79"/>
-      <c r="C55" s="79"/>
+      <c r="B55" s="72"/>
+      <c r="C55" s="72"/>
       <c r="F55" s="41"/>
       <c r="H55" s="42"/>
       <c r="J55" s="42"/>
@@ -7195,36 +7209,36 @@
       <c r="Q55" s="42"/>
     </row>
     <row r="56" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A56" s="73" t="s">
+      <c r="A56" s="74" t="s">
         <v>47</v>
       </c>
-      <c r="B56" s="73"/>
-      <c r="C56" s="73"/>
-      <c r="D56" s="73"/>
-      <c r="E56" s="73"/>
-      <c r="F56" s="73"/>
-      <c r="G56" s="74"/>
-      <c r="H56" s="75" t="s">
+      <c r="B56" s="74"/>
+      <c r="C56" s="74"/>
+      <c r="D56" s="74"/>
+      <c r="E56" s="74"/>
+      <c r="F56" s="74"/>
+      <c r="G56" s="75"/>
+      <c r="H56" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="I56" s="76"/>
-      <c r="J56" s="75" t="s">
+      <c r="I56" s="77"/>
+      <c r="J56" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="K56" s="76"/>
-      <c r="L56" s="75" t="s">
+      <c r="K56" s="77"/>
+      <c r="L56" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="M56" s="76"/>
+      <c r="M56" s="77"/>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B57" s="77" t="s">
+      <c r="B57" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="C57" s="77"/>
+      <c r="C57" s="79"/>
       <c r="D57" s="26" t="s">
         <v>1</v>
       </c>
@@ -7260,10 +7274,10 @@
       <c r="A58" s="35">
         <v>12</v>
       </c>
-      <c r="B58" s="78" t="s">
+      <c r="B58" s="80" t="s">
         <v>48</v>
       </c>
-      <c r="C58" s="78"/>
+      <c r="C58" s="80"/>
       <c r="D58" s="34" t="s">
         <v>49</v>
       </c>
@@ -7285,7 +7299,7 @@
       </c>
       <c r="K58" s="31"/>
       <c r="L58" s="31" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="M58" s="31"/>
     </row>
@@ -7293,18 +7307,18 @@
       <c r="A59" s="35">
         <v>13</v>
       </c>
-      <c r="B59" s="80" t="s">
+      <c r="B59" s="81" t="s">
         <v>48</v>
       </c>
-      <c r="C59" s="80"/>
+      <c r="C59" s="81"/>
       <c r="D59" s="34" t="s">
         <v>81</v>
       </c>
       <c r="E59" s="32" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F59" s="29" t="s">
-        <v>82</v>
+        <v>156</v>
       </c>
       <c r="G59" s="35" t="s">
         <v>32</v>
@@ -7318,9 +7332,11 @@
       </c>
       <c r="K59" s="31"/>
       <c r="L59" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="M59" s="31"/>
+        <v>12</v>
+      </c>
+      <c r="M59" s="69" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B60" s="70"/>
@@ -7334,22 +7350,22 @@
       <c r="B61" s="70"/>
       <c r="C61" s="70"/>
       <c r="F61" s="13"/>
-      <c r="H61" s="72" t="s">
+      <c r="H61" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="I61" s="72"/>
-      <c r="J61" s="72"/>
-      <c r="K61" s="72"/>
-      <c r="L61" s="72"/>
-      <c r="M61" s="72"/>
-      <c r="O61" s="72" t="s">
-        <v>83</v>
-      </c>
-      <c r="P61" s="72"/>
-      <c r="Q61" s="72"/>
-      <c r="R61" s="72"/>
-      <c r="S61" s="72"/>
-      <c r="T61" s="72"/>
+      <c r="I61" s="73"/>
+      <c r="J61" s="73"/>
+      <c r="K61" s="73"/>
+      <c r="L61" s="73"/>
+      <c r="M61" s="73"/>
+      <c r="O61" s="73" t="s">
+        <v>82</v>
+      </c>
+      <c r="P61" s="73"/>
+      <c r="Q61" s="73"/>
+      <c r="R61" s="73"/>
+      <c r="S61" s="73"/>
+      <c r="T61" s="73"/>
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B62" s="70"/>
@@ -7467,14 +7483,14 @@
       <c r="K65" s="71"/>
       <c r="L65" s="71"/>
       <c r="M65" s="71"/>
-      <c r="O65" s="72" t="s">
-        <v>84</v>
-      </c>
-      <c r="P65" s="72"/>
-      <c r="Q65" s="72"/>
-      <c r="R65" s="72"/>
-      <c r="S65" s="72"/>
-      <c r="T65" s="72"/>
+      <c r="O65" s="73" t="s">
+        <v>83</v>
+      </c>
+      <c r="P65" s="73"/>
+      <c r="Q65" s="73"/>
+      <c r="R65" s="73"/>
+      <c r="S65" s="73"/>
+      <c r="T65" s="73"/>
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B66" s="70"/>
@@ -7523,7 +7539,7 @@
       <c r="F67" s="13"/>
       <c r="H67" s="14">
         <f>H63+O63+O67</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I67" s="14">
         <f>I63+P63+P67</f>
@@ -7535,7 +7551,7 @@
       </c>
       <c r="K67" s="14">
         <f>K63+R63+R67</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L67" s="14">
         <f>SUM(H67:K67)</f>
@@ -7543,11 +7559,11 @@
       </c>
       <c r="M67" s="15">
         <f>(K67+I67)/L67</f>
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
       <c r="O67" s="14">
         <f>COUNTIF(L58:L59,"O")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P67" s="14">
         <f>COUNTIF(J61:J63,"N")</f>
@@ -7559,7 +7575,7 @@
       </c>
       <c r="R67" s="14">
         <f>COUNTIF(L58:L59,"R")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S67" s="14">
         <f>SUM(O67:R67)</f>
@@ -7567,13 +7583,13 @@
       </c>
       <c r="T67" s="15">
         <f>(R67+P67)/S67</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" s="40"/>
-      <c r="B68" s="79"/>
-      <c r="C68" s="79"/>
+      <c r="B68" s="72"/>
+      <c r="C68" s="72"/>
       <c r="D68" s="40"/>
       <c r="E68" s="40"/>
       <c r="F68" s="41"/>
@@ -7587,27 +7603,27 @@
       <c r="N68" s="40"/>
     </row>
     <row r="69" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A69" s="73" t="s">
+      <c r="A69" s="74" t="s">
         <v>52</v>
       </c>
-      <c r="B69" s="73"/>
-      <c r="C69" s="73"/>
-      <c r="D69" s="73"/>
-      <c r="E69" s="73"/>
-      <c r="F69" s="73"/>
-      <c r="G69" s="74"/>
-      <c r="H69" s="75" t="s">
+      <c r="B69" s="74"/>
+      <c r="C69" s="74"/>
+      <c r="D69" s="74"/>
+      <c r="E69" s="74"/>
+      <c r="F69" s="74"/>
+      <c r="G69" s="75"/>
+      <c r="H69" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="I69" s="76"/>
-      <c r="J69" s="75" t="s">
+      <c r="I69" s="77"/>
+      <c r="J69" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="K69" s="76"/>
-      <c r="L69" s="75" t="s">
+      <c r="K69" s="77"/>
+      <c r="L69" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="M69" s="76"/>
+      <c r="M69" s="77"/>
       <c r="O69" s="37"/>
       <c r="Q69" s="37"/>
     </row>
@@ -7615,10 +7631,10 @@
       <c r="A70" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B70" s="77" t="s">
+      <c r="B70" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="C70" s="77"/>
+      <c r="C70" s="79"/>
       <c r="D70" s="38" t="s">
         <v>1</v>
       </c>
@@ -7656,10 +7672,10 @@
       <c r="A71" s="39">
         <v>14</v>
       </c>
-      <c r="B71" s="78" t="s">
+      <c r="B71" s="80" t="s">
         <v>53</v>
       </c>
-      <c r="C71" s="78"/>
+      <c r="C71" s="80"/>
       <c r="D71" s="34" t="s">
         <v>54</v>
       </c>
@@ -7681,7 +7697,7 @@
       </c>
       <c r="K71" s="31"/>
       <c r="L71" s="31" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="M71" s="31"/>
       <c r="O71" s="37"/>
@@ -7701,22 +7717,22 @@
       <c r="B73" s="70"/>
       <c r="C73" s="70"/>
       <c r="F73" s="13"/>
-      <c r="H73" s="72" t="s">
+      <c r="H73" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="I73" s="72"/>
-      <c r="J73" s="72"/>
-      <c r="K73" s="72"/>
-      <c r="L73" s="72"/>
-      <c r="M73" s="72"/>
-      <c r="O73" s="72" t="s">
-        <v>83</v>
-      </c>
-      <c r="P73" s="72"/>
-      <c r="Q73" s="72"/>
-      <c r="R73" s="72"/>
-      <c r="S73" s="72"/>
-      <c r="T73" s="72"/>
+      <c r="I73" s="73"/>
+      <c r="J73" s="73"/>
+      <c r="K73" s="73"/>
+      <c r="L73" s="73"/>
+      <c r="M73" s="73"/>
+      <c r="O73" s="73" t="s">
+        <v>82</v>
+      </c>
+      <c r="P73" s="73"/>
+      <c r="Q73" s="73"/>
+      <c r="R73" s="73"/>
+      <c r="S73" s="73"/>
+      <c r="T73" s="73"/>
     </row>
     <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B74" s="70"/>
@@ -7834,14 +7850,14 @@
       <c r="K77" s="71"/>
       <c r="L77" s="71"/>
       <c r="M77" s="71"/>
-      <c r="O77" s="72" t="s">
-        <v>84</v>
-      </c>
-      <c r="P77" s="72"/>
-      <c r="Q77" s="72"/>
-      <c r="R77" s="72"/>
-      <c r="S77" s="72"/>
-      <c r="T77" s="72"/>
+      <c r="O77" s="73" t="s">
+        <v>83</v>
+      </c>
+      <c r="P77" s="73"/>
+      <c r="Q77" s="73"/>
+      <c r="R77" s="73"/>
+      <c r="S77" s="73"/>
+      <c r="T77" s="73"/>
     </row>
     <row r="78" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B78" s="70"/>
@@ -7890,7 +7906,7 @@
       <c r="F79" s="13"/>
       <c r="H79" s="14">
         <f>H75+O75+O79</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I79" s="14">
         <f>I75+P75+P79</f>
@@ -7902,7 +7918,7 @@
       </c>
       <c r="K79" s="14">
         <f>K75+R75+R79</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L79" s="14">
         <f>SUM(H79:K79)</f>
@@ -7910,11 +7926,11 @@
       </c>
       <c r="M79" s="15">
         <f>(K79+I79)/L79</f>
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
       <c r="O79" s="14">
         <f>COUNTIF(L69:L71,"O")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P79" s="14">
         <f>COUNTIF(J73:J75,"N")</f>
@@ -7926,7 +7942,7 @@
       </c>
       <c r="R79" s="14">
         <f>COUNTIF(L69:L71,"R")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S79" s="14">
         <f>SUM(O79:R79)</f>
@@ -7934,13 +7950,13 @@
       </c>
       <c r="T79" s="15">
         <f>(R79+P79)/S79</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A80" s="40"/>
-      <c r="B80" s="79"/>
-      <c r="C80" s="79"/>
+      <c r="B80" s="72"/>
+      <c r="C80" s="72"/>
       <c r="D80" s="40"/>
       <c r="E80" s="40"/>
       <c r="F80" s="41"/>
@@ -7956,27 +7972,27 @@
       <c r="Q80" s="37"/>
     </row>
     <row r="81" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A81" s="73" t="s">
+      <c r="A81" s="74" t="s">
         <v>57</v>
       </c>
-      <c r="B81" s="73"/>
-      <c r="C81" s="73"/>
-      <c r="D81" s="73"/>
-      <c r="E81" s="73"/>
-      <c r="F81" s="73"/>
-      <c r="G81" s="74"/>
-      <c r="H81" s="75" t="s">
+      <c r="B81" s="74"/>
+      <c r="C81" s="74"/>
+      <c r="D81" s="74"/>
+      <c r="E81" s="74"/>
+      <c r="F81" s="74"/>
+      <c r="G81" s="75"/>
+      <c r="H81" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="I81" s="76"/>
-      <c r="J81" s="75" t="s">
+      <c r="I81" s="77"/>
+      <c r="J81" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="K81" s="76"/>
-      <c r="L81" s="75" t="s">
+      <c r="K81" s="77"/>
+      <c r="L81" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="M81" s="76"/>
+      <c r="M81" s="77"/>
       <c r="O81" s="37"/>
       <c r="Q81" s="37"/>
     </row>
@@ -7984,10 +8000,10 @@
       <c r="A82" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B82" s="77" t="s">
+      <c r="B82" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="C82" s="77"/>
+      <c r="C82" s="79"/>
       <c r="D82" s="38" t="s">
         <v>1</v>
       </c>
@@ -8025,10 +8041,10 @@
       <c r="A83" s="39">
         <v>15</v>
       </c>
-      <c r="B83" s="78" t="s">
+      <c r="B83" s="80" t="s">
         <v>58</v>
       </c>
-      <c r="C83" s="78"/>
+      <c r="C83" s="80"/>
       <c r="D83" s="34" t="s">
         <v>59</v>
       </c>
@@ -8050,7 +8066,7 @@
       </c>
       <c r="K83" s="31"/>
       <c r="L83" s="31" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="M83" s="31"/>
       <c r="O83" s="37"/>
@@ -8070,22 +8086,22 @@
       <c r="B85" s="70"/>
       <c r="C85" s="70"/>
       <c r="F85" s="13"/>
-      <c r="H85" s="72" t="s">
+      <c r="H85" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="I85" s="72"/>
-      <c r="J85" s="72"/>
-      <c r="K85" s="72"/>
-      <c r="L85" s="72"/>
-      <c r="M85" s="72"/>
-      <c r="O85" s="72" t="s">
-        <v>83</v>
-      </c>
-      <c r="P85" s="72"/>
-      <c r="Q85" s="72"/>
-      <c r="R85" s="72"/>
-      <c r="S85" s="72"/>
-      <c r="T85" s="72"/>
+      <c r="I85" s="73"/>
+      <c r="J85" s="73"/>
+      <c r="K85" s="73"/>
+      <c r="L85" s="73"/>
+      <c r="M85" s="73"/>
+      <c r="O85" s="73" t="s">
+        <v>82</v>
+      </c>
+      <c r="P85" s="73"/>
+      <c r="Q85" s="73"/>
+      <c r="R85" s="73"/>
+      <c r="S85" s="73"/>
+      <c r="T85" s="73"/>
     </row>
     <row r="86" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B86" s="70"/>
@@ -8203,14 +8219,14 @@
       <c r="K89" s="71"/>
       <c r="L89" s="71"/>
       <c r="M89" s="71"/>
-      <c r="O89" s="72" t="s">
-        <v>84</v>
-      </c>
-      <c r="P89" s="72"/>
-      <c r="Q89" s="72"/>
-      <c r="R89" s="72"/>
-      <c r="S89" s="72"/>
-      <c r="T89" s="72"/>
+      <c r="O89" s="73" t="s">
+        <v>83</v>
+      </c>
+      <c r="P89" s="73"/>
+      <c r="Q89" s="73"/>
+      <c r="R89" s="73"/>
+      <c r="S89" s="73"/>
+      <c r="T89" s="73"/>
     </row>
     <row r="90" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B90" s="70"/>
@@ -8259,7 +8275,7 @@
       <c r="F91" s="13"/>
       <c r="H91" s="14">
         <f>H87+O87+O91</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I91" s="14">
         <f>I87+P87+P91</f>
@@ -8271,7 +8287,7 @@
       </c>
       <c r="K91" s="14">
         <f>K87+R87+R91</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L91" s="14">
         <f>SUM(H91:K91)</f>
@@ -8279,11 +8295,11 @@
       </c>
       <c r="M91" s="15">
         <f>(K91+I91)/L91</f>
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
       <c r="O91" s="14">
         <f>COUNTIF(L81:L83,"O")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P91" s="14">
         <f>COUNTIF(J85:J87,"N")</f>
@@ -8295,7 +8311,7 @@
       </c>
       <c r="R91" s="14">
         <f>COUNTIF(L81:L83,"R")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S91" s="14">
         <f>SUM(O91:R91)</f>
@@ -8303,13 +8319,13 @@
       </c>
       <c r="T91" s="15">
         <f>(R91+P91)/S91</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A92" s="40"/>
-      <c r="B92" s="79"/>
-      <c r="C92" s="79"/>
+      <c r="B92" s="72"/>
+      <c r="C92" s="72"/>
       <c r="D92" s="40"/>
       <c r="E92" s="40"/>
       <c r="F92" s="41"/>
@@ -8325,27 +8341,27 @@
       <c r="Q92" s="37"/>
     </row>
     <row r="93" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A93" s="73" t="s">
-        <v>92</v>
-      </c>
-      <c r="B93" s="73"/>
-      <c r="C93" s="73"/>
-      <c r="D93" s="73"/>
-      <c r="E93" s="73"/>
-      <c r="F93" s="73"/>
-      <c r="G93" s="74"/>
-      <c r="H93" s="75" t="s">
+      <c r="A93" s="74" t="s">
+        <v>91</v>
+      </c>
+      <c r="B93" s="74"/>
+      <c r="C93" s="74"/>
+      <c r="D93" s="74"/>
+      <c r="E93" s="74"/>
+      <c r="F93" s="74"/>
+      <c r="G93" s="75"/>
+      <c r="H93" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="I93" s="76"/>
-      <c r="J93" s="75" t="s">
+      <c r="I93" s="77"/>
+      <c r="J93" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="K93" s="76"/>
-      <c r="L93" s="75" t="s">
+      <c r="K93" s="77"/>
+      <c r="L93" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="M93" s="76"/>
+      <c r="M93" s="77"/>
       <c r="O93" s="37"/>
       <c r="Q93" s="37"/>
     </row>
@@ -8353,10 +8369,10 @@
       <c r="A94" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B94" s="77" t="s">
+      <c r="B94" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="C94" s="77"/>
+      <c r="C94" s="79"/>
       <c r="D94" s="38" t="s">
         <v>1</v>
       </c>
@@ -8394,18 +8410,18 @@
       <c r="A95" s="39">
         <v>16</v>
       </c>
-      <c r="B95" s="78" t="s">
+      <c r="B95" s="80" t="s">
         <v>62</v>
       </c>
-      <c r="C95" s="78"/>
+      <c r="C95" s="80"/>
       <c r="D95" s="50" t="s">
+        <v>92</v>
+      </c>
+      <c r="E95" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="E95" s="32" t="s">
+      <c r="F95" s="29" t="s">
         <v>94</v>
-      </c>
-      <c r="F95" s="29" t="s">
-        <v>95</v>
       </c>
       <c r="G95" s="39" t="s">
         <v>32</v>
@@ -8419,7 +8435,7 @@
       </c>
       <c r="K95" s="31"/>
       <c r="L95" s="31" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="M95" s="31"/>
       <c r="O95" s="37"/>
@@ -8429,18 +8445,18 @@
       <c r="A96" s="39">
         <v>17</v>
       </c>
-      <c r="B96" s="80" t="s">
+      <c r="B96" s="81" t="s">
         <v>62</v>
       </c>
-      <c r="C96" s="80"/>
+      <c r="C96" s="81"/>
       <c r="D96" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="E96" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="F96" s="29" t="s">
         <v>126</v>
-      </c>
-      <c r="E96" s="32" t="s">
-        <v>96</v>
-      </c>
-      <c r="F96" s="29" t="s">
-        <v>127</v>
       </c>
       <c r="G96" s="39" t="s">
         <v>32</v>
@@ -8454,7 +8470,7 @@
       </c>
       <c r="K96" s="31"/>
       <c r="L96" s="31" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="M96" s="31"/>
       <c r="O96" s="37"/>
@@ -8474,22 +8490,22 @@
       <c r="B98" s="70"/>
       <c r="C98" s="70"/>
       <c r="F98" s="13"/>
-      <c r="H98" s="72" t="s">
+      <c r="H98" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="I98" s="72"/>
-      <c r="J98" s="72"/>
-      <c r="K98" s="72"/>
-      <c r="L98" s="72"/>
-      <c r="M98" s="72"/>
-      <c r="O98" s="72" t="s">
-        <v>83</v>
-      </c>
-      <c r="P98" s="72"/>
-      <c r="Q98" s="72"/>
-      <c r="R98" s="72"/>
-      <c r="S98" s="72"/>
-      <c r="T98" s="72"/>
+      <c r="I98" s="73"/>
+      <c r="J98" s="73"/>
+      <c r="K98" s="73"/>
+      <c r="L98" s="73"/>
+      <c r="M98" s="73"/>
+      <c r="O98" s="73" t="s">
+        <v>82</v>
+      </c>
+      <c r="P98" s="73"/>
+      <c r="Q98" s="73"/>
+      <c r="R98" s="73"/>
+      <c r="S98" s="73"/>
+      <c r="T98" s="73"/>
     </row>
     <row r="99" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B99" s="70"/>
@@ -8607,14 +8623,14 @@
       <c r="K102" s="71"/>
       <c r="L102" s="71"/>
       <c r="M102" s="71"/>
-      <c r="O102" s="72" t="s">
-        <v>84</v>
-      </c>
-      <c r="P102" s="72"/>
-      <c r="Q102" s="72"/>
-      <c r="R102" s="72"/>
-      <c r="S102" s="72"/>
-      <c r="T102" s="72"/>
+      <c r="O102" s="73" t="s">
+        <v>83</v>
+      </c>
+      <c r="P102" s="73"/>
+      <c r="Q102" s="73"/>
+      <c r="R102" s="73"/>
+      <c r="S102" s="73"/>
+      <c r="T102" s="73"/>
     </row>
     <row r="103" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B103" s="70"/>
@@ -8663,7 +8679,7 @@
       <c r="F104" s="13"/>
       <c r="H104" s="14">
         <f>H100+O100+O104</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I104" s="14">
         <f>I100+P100+P104</f>
@@ -8675,7 +8691,7 @@
       </c>
       <c r="K104" s="14">
         <f>K100+R100+R104</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L104" s="14">
         <f>SUM(H104:K104)</f>
@@ -8683,11 +8699,11 @@
       </c>
       <c r="M104" s="15">
         <f>(K104+I104)/L104</f>
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
       <c r="O104" s="14">
         <f>COUNTIF(L95:L96,"O")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P104" s="14">
         <f>COUNTIF(J98:J100,"N")</f>
@@ -8699,7 +8715,7 @@
       </c>
       <c r="R104" s="14">
         <f>COUNTIF(L95:L96,"R")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S104" s="14">
         <f>SUM(O104:R104)</f>
@@ -8707,13 +8723,13 @@
       </c>
       <c r="T104" s="15">
         <f>(R104+P104)/S104</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A105" s="40"/>
-      <c r="B105" s="79"/>
-      <c r="C105" s="79"/>
+      <c r="B105" s="72"/>
+      <c r="C105" s="72"/>
       <c r="D105" s="40"/>
       <c r="E105" s="40"/>
       <c r="F105" s="41"/>
@@ -8729,27 +8745,27 @@
       <c r="Q105" s="37"/>
     </row>
     <row r="106" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A106" s="73" t="s">
-        <v>104</v>
-      </c>
-      <c r="B106" s="73"/>
-      <c r="C106" s="73"/>
-      <c r="D106" s="73"/>
-      <c r="E106" s="73"/>
-      <c r="F106" s="73"/>
-      <c r="G106" s="74"/>
-      <c r="H106" s="75" t="s">
+      <c r="A106" s="74" t="s">
+        <v>103</v>
+      </c>
+      <c r="B106" s="74"/>
+      <c r="C106" s="74"/>
+      <c r="D106" s="74"/>
+      <c r="E106" s="74"/>
+      <c r="F106" s="74"/>
+      <c r="G106" s="75"/>
+      <c r="H106" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="I106" s="76"/>
-      <c r="J106" s="75" t="s">
+      <c r="I106" s="77"/>
+      <c r="J106" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="K106" s="76"/>
-      <c r="L106" s="75" t="s">
+      <c r="K106" s="77"/>
+      <c r="L106" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="M106" s="76"/>
+      <c r="M106" s="77"/>
       <c r="O106" s="46"/>
       <c r="Q106" s="46"/>
     </row>
@@ -8757,10 +8773,10 @@
       <c r="A107" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B107" s="77" t="s">
+      <c r="B107" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="C107" s="77"/>
+      <c r="C107" s="79"/>
       <c r="D107" s="49" t="s">
         <v>1</v>
       </c>
@@ -8798,18 +8814,18 @@
       <c r="A108" s="48">
         <v>18</v>
       </c>
-      <c r="B108" s="78" t="s">
-        <v>106</v>
-      </c>
-      <c r="C108" s="78"/>
+      <c r="B108" s="80" t="s">
+        <v>105</v>
+      </c>
+      <c r="C108" s="80"/>
       <c r="D108" s="50" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E108" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="F108" s="29" t="s">
         <v>97</v>
-      </c>
-      <c r="F108" s="29" t="s">
-        <v>98</v>
       </c>
       <c r="G108" s="48" t="s">
         <v>32</v>
@@ -8823,7 +8839,7 @@
       </c>
       <c r="K108" s="31"/>
       <c r="L108" s="31" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="M108" s="31"/>
       <c r="O108" s="46"/>
@@ -8833,18 +8849,18 @@
       <c r="A109" s="68">
         <v>19</v>
       </c>
-      <c r="B109" s="80" t="s">
-        <v>106</v>
-      </c>
-      <c r="C109" s="80"/>
+      <c r="B109" s="81" t="s">
+        <v>105</v>
+      </c>
+      <c r="C109" s="81"/>
       <c r="D109" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="E109" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="F109" s="29" t="s">
         <v>129</v>
-      </c>
-      <c r="E109" s="32" t="s">
-        <v>96</v>
-      </c>
-      <c r="F109" s="29" t="s">
-        <v>130</v>
       </c>
       <c r="G109" s="48" t="s">
         <v>32</v>
@@ -8858,7 +8874,7 @@
       </c>
       <c r="K109" s="31"/>
       <c r="L109" s="31" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="M109" s="31"/>
       <c r="O109" s="46"/>
@@ -8878,22 +8894,22 @@
       <c r="B111" s="70"/>
       <c r="C111" s="70"/>
       <c r="F111" s="13"/>
-      <c r="H111" s="72" t="s">
+      <c r="H111" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="I111" s="72"/>
-      <c r="J111" s="72"/>
-      <c r="K111" s="72"/>
-      <c r="L111" s="72"/>
-      <c r="M111" s="72"/>
-      <c r="O111" s="72" t="s">
-        <v>83</v>
-      </c>
-      <c r="P111" s="72"/>
-      <c r="Q111" s="72"/>
-      <c r="R111" s="72"/>
-      <c r="S111" s="72"/>
-      <c r="T111" s="72"/>
+      <c r="I111" s="73"/>
+      <c r="J111" s="73"/>
+      <c r="K111" s="73"/>
+      <c r="L111" s="73"/>
+      <c r="M111" s="73"/>
+      <c r="O111" s="73" t="s">
+        <v>82</v>
+      </c>
+      <c r="P111" s="73"/>
+      <c r="Q111" s="73"/>
+      <c r="R111" s="73"/>
+      <c r="S111" s="73"/>
+      <c r="T111" s="73"/>
     </row>
     <row r="112" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B112" s="70"/>
@@ -9011,14 +9027,14 @@
       <c r="K115" s="71"/>
       <c r="L115" s="71"/>
       <c r="M115" s="71"/>
-      <c r="O115" s="72" t="s">
-        <v>84</v>
-      </c>
-      <c r="P115" s="72"/>
-      <c r="Q115" s="72"/>
-      <c r="R115" s="72"/>
-      <c r="S115" s="72"/>
-      <c r="T115" s="72"/>
+      <c r="O115" s="73" t="s">
+        <v>83</v>
+      </c>
+      <c r="P115" s="73"/>
+      <c r="Q115" s="73"/>
+      <c r="R115" s="73"/>
+      <c r="S115" s="73"/>
+      <c r="T115" s="73"/>
     </row>
     <row r="116" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B116" s="70"/>
@@ -9067,7 +9083,7 @@
       <c r="F117" s="13"/>
       <c r="H117" s="14">
         <f>H113+O113+O117</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I117" s="14">
         <f>I113+P113+P117</f>
@@ -9079,7 +9095,7 @@
       </c>
       <c r="K117" s="14">
         <f>K113+R113+R117</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L117" s="14">
         <f>SUM(H117:K117)</f>
@@ -9087,11 +9103,11 @@
       </c>
       <c r="M117" s="15">
         <f>(K117+I117)/L117</f>
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
       <c r="O117" s="14">
         <f>COUNTIF(L108:L109,"O")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P117" s="14">
         <f>COUNTIF(J111:J113,"N")</f>
@@ -9103,7 +9119,7 @@
       </c>
       <c r="R117" s="14">
         <f>COUNTIF(L108:L109,"R")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S117" s="14">
         <f>SUM(O117:R117)</f>
@@ -9111,7 +9127,7 @@
       </c>
       <c r="T117" s="15">
         <f>(R117+P117)/S117</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="118" spans="1:20" x14ac:dyDescent="0.25">
@@ -9132,27 +9148,27 @@
       <c r="T118" s="62"/>
     </row>
     <row r="119" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A119" s="73" t="s">
-        <v>145</v>
-      </c>
-      <c r="B119" s="73"/>
-      <c r="C119" s="73"/>
-      <c r="D119" s="73"/>
-      <c r="E119" s="73"/>
-      <c r="F119" s="73"/>
-      <c r="G119" s="74"/>
-      <c r="H119" s="75" t="s">
+      <c r="A119" s="74" t="s">
+        <v>144</v>
+      </c>
+      <c r="B119" s="74"/>
+      <c r="C119" s="74"/>
+      <c r="D119" s="74"/>
+      <c r="E119" s="74"/>
+      <c r="F119" s="74"/>
+      <c r="G119" s="75"/>
+      <c r="H119" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="I119" s="76"/>
-      <c r="J119" s="75" t="s">
+      <c r="I119" s="77"/>
+      <c r="J119" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="K119" s="76"/>
-      <c r="L119" s="75" t="s">
+      <c r="K119" s="77"/>
+      <c r="L119" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="M119" s="76"/>
+      <c r="M119" s="77"/>
       <c r="O119" s="63"/>
       <c r="Q119" s="63"/>
     </row>
@@ -9160,10 +9176,10 @@
       <c r="A120" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="B120" s="77" t="s">
+      <c r="B120" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="C120" s="77"/>
+      <c r="C120" s="79"/>
       <c r="D120" s="66" t="s">
         <v>1</v>
       </c>
@@ -9201,18 +9217,18 @@
       <c r="A121" s="65">
         <v>20</v>
       </c>
-      <c r="B121" s="78" t="s">
+      <c r="B121" s="80" t="s">
+        <v>145</v>
+      </c>
+      <c r="C121" s="80"/>
+      <c r="D121" s="50" t="s">
+        <v>147</v>
+      </c>
+      <c r="E121" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="F121" s="29" t="s">
         <v>146</v>
-      </c>
-      <c r="C121" s="78"/>
-      <c r="D121" s="50" t="s">
-        <v>148</v>
-      </c>
-      <c r="E121" s="32" t="s">
-        <v>97</v>
-      </c>
-      <c r="F121" s="29" t="s">
-        <v>147</v>
       </c>
       <c r="G121" s="65" t="s">
         <v>32</v>
@@ -9226,9 +9242,11 @@
       </c>
       <c r="K121" s="31"/>
       <c r="L121" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="M121" s="31"/>
+        <v>12</v>
+      </c>
+      <c r="M121" s="31" t="s">
+        <v>157</v>
+      </c>
       <c r="O121" s="63"/>
       <c r="Q121" s="63"/>
     </row>
@@ -9246,28 +9264,28 @@
       <c r="B123" s="70"/>
       <c r="C123" s="70"/>
       <c r="F123" s="13"/>
-      <c r="H123" s="72" t="s">
+      <c r="H123" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="I123" s="72"/>
-      <c r="J123" s="72"/>
-      <c r="K123" s="72"/>
-      <c r="L123" s="72"/>
-      <c r="M123" s="72"/>
-      <c r="O123" s="72" t="s">
-        <v>83</v>
-      </c>
-      <c r="P123" s="72"/>
-      <c r="Q123" s="72"/>
-      <c r="R123" s="72"/>
-      <c r="S123" s="72"/>
-      <c r="T123" s="72"/>
+      <c r="I123" s="73"/>
+      <c r="J123" s="73"/>
+      <c r="K123" s="73"/>
+      <c r="L123" s="73"/>
+      <c r="M123" s="73"/>
+      <c r="O123" s="73" t="s">
+        <v>82</v>
+      </c>
+      <c r="P123" s="73"/>
+      <c r="Q123" s="73"/>
+      <c r="R123" s="73"/>
+      <c r="S123" s="73"/>
+      <c r="T123" s="73"/>
     </row>
     <row r="124" spans="1:20" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B124" s="70"/>
       <c r="C124" s="70"/>
       <c r="E124" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F124" s="13"/>
       <c r="H124" s="16" t="s">
@@ -9382,14 +9400,14 @@
       <c r="K127" s="71"/>
       <c r="L127" s="71"/>
       <c r="M127" s="71"/>
-      <c r="O127" s="72" t="s">
-        <v>84</v>
-      </c>
-      <c r="P127" s="72"/>
-      <c r="Q127" s="72"/>
-      <c r="R127" s="72"/>
-      <c r="S127" s="72"/>
-      <c r="T127" s="72"/>
+      <c r="O127" s="73" t="s">
+        <v>83</v>
+      </c>
+      <c r="P127" s="73"/>
+      <c r="Q127" s="73"/>
+      <c r="R127" s="73"/>
+      <c r="S127" s="73"/>
+      <c r="T127" s="73"/>
     </row>
     <row r="128" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B128" s="70"/>
@@ -9438,7 +9456,7 @@
       <c r="F129" s="13"/>
       <c r="H129" s="14">
         <f>H125+O125+O129</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I129" s="14">
         <f>I125+P125+P129</f>
@@ -9450,7 +9468,7 @@
       </c>
       <c r="K129" s="14">
         <f>K125+R125+R129</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L129" s="14">
         <f>SUM(H129:K129)</f>
@@ -9458,11 +9476,11 @@
       </c>
       <c r="M129" s="15">
         <f>(K129+I129)/L129</f>
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
       <c r="O129" s="14">
         <f>COUNTIF(L121:L121,"O")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P129" s="14">
         <f>COUNTIF(J123:J125,"N")</f>
@@ -9474,7 +9492,7 @@
       </c>
       <c r="R129" s="14">
         <f>COUNTIF(L121:L121,"R")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S129" s="14">
         <f>SUM(O129:R129)</f>
@@ -9482,7 +9500,7 @@
       </c>
       <c r="T129" s="15">
         <f>(R129+P129)/S129</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="130" spans="1:20" x14ac:dyDescent="0.25">
@@ -9503,27 +9521,27 @@
       <c r="T130" s="62"/>
     </row>
     <row r="131" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A131" s="73" t="s">
-        <v>103</v>
-      </c>
-      <c r="B131" s="73"/>
-      <c r="C131" s="73"/>
-      <c r="D131" s="73"/>
-      <c r="E131" s="73"/>
-      <c r="F131" s="73"/>
-      <c r="G131" s="74"/>
-      <c r="H131" s="75" t="s">
+      <c r="A131" s="74" t="s">
+        <v>102</v>
+      </c>
+      <c r="B131" s="74"/>
+      <c r="C131" s="74"/>
+      <c r="D131" s="74"/>
+      <c r="E131" s="74"/>
+      <c r="F131" s="74"/>
+      <c r="G131" s="75"/>
+      <c r="H131" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="I131" s="76"/>
-      <c r="J131" s="75" t="s">
+      <c r="I131" s="77"/>
+      <c r="J131" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="K131" s="76"/>
-      <c r="L131" s="75" t="s">
+      <c r="K131" s="77"/>
+      <c r="L131" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="M131" s="76"/>
+      <c r="M131" s="77"/>
       <c r="O131" s="52"/>
       <c r="Q131" s="52"/>
     </row>
@@ -9531,10 +9549,10 @@
       <c r="A132" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B132" s="77" t="s">
+      <c r="B132" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="C132" s="77"/>
+      <c r="C132" s="79"/>
       <c r="D132" s="55" t="s">
         <v>1</v>
       </c>
@@ -9572,18 +9590,18 @@
       <c r="A133" s="54">
         <v>21</v>
       </c>
-      <c r="B133" s="78" t="s">
-        <v>105</v>
-      </c>
-      <c r="C133" s="78"/>
+      <c r="B133" s="80" t="s">
+        <v>104</v>
+      </c>
+      <c r="C133" s="80"/>
       <c r="D133" s="50" t="s">
+        <v>106</v>
+      </c>
+      <c r="E133" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="E133" s="32" t="s">
+      <c r="F133" s="29" t="s">
         <v>108</v>
-      </c>
-      <c r="F133" s="29" t="s">
-        <v>109</v>
       </c>
       <c r="G133" s="54" t="s">
         <v>32</v>
@@ -9597,7 +9615,7 @@
       </c>
       <c r="K133" s="31"/>
       <c r="L133" s="31" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="M133" s="31"/>
       <c r="O133" s="52"/>
@@ -9607,18 +9625,18 @@
       <c r="A134" s="54">
         <v>22</v>
       </c>
-      <c r="B134" s="80" t="s">
-        <v>105</v>
-      </c>
-      <c r="C134" s="80"/>
+      <c r="B134" s="81" t="s">
+        <v>104</v>
+      </c>
+      <c r="C134" s="81"/>
       <c r="D134" s="50" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E134" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="F134" s="29" t="s">
         <v>110</v>
-      </c>
-      <c r="F134" s="29" t="s">
-        <v>111</v>
       </c>
       <c r="G134" s="54" t="s">
         <v>32</v>
@@ -9632,7 +9650,7 @@
       </c>
       <c r="K134" s="31"/>
       <c r="L134" s="31" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="M134" s="31"/>
       <c r="O134" s="52"/>
@@ -9652,22 +9670,22 @@
       <c r="B136" s="70"/>
       <c r="C136" s="70"/>
       <c r="F136" s="13"/>
-      <c r="H136" s="72" t="s">
+      <c r="H136" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="I136" s="72"/>
-      <c r="J136" s="72"/>
-      <c r="K136" s="72"/>
-      <c r="L136" s="72"/>
-      <c r="M136" s="72"/>
-      <c r="O136" s="72" t="s">
-        <v>83</v>
-      </c>
-      <c r="P136" s="72"/>
-      <c r="Q136" s="72"/>
-      <c r="R136" s="72"/>
-      <c r="S136" s="72"/>
-      <c r="T136" s="72"/>
+      <c r="I136" s="73"/>
+      <c r="J136" s="73"/>
+      <c r="K136" s="73"/>
+      <c r="L136" s="73"/>
+      <c r="M136" s="73"/>
+      <c r="O136" s="73" t="s">
+        <v>82</v>
+      </c>
+      <c r="P136" s="73"/>
+      <c r="Q136" s="73"/>
+      <c r="R136" s="73"/>
+      <c r="S136" s="73"/>
+      <c r="T136" s="73"/>
     </row>
     <row r="137" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B137" s="70"/>
@@ -9785,14 +9803,14 @@
       <c r="K140" s="71"/>
       <c r="L140" s="71"/>
       <c r="M140" s="71"/>
-      <c r="O140" s="72" t="s">
-        <v>84</v>
-      </c>
-      <c r="P140" s="72"/>
-      <c r="Q140" s="72"/>
-      <c r="R140" s="72"/>
-      <c r="S140" s="72"/>
-      <c r="T140" s="72"/>
+      <c r="O140" s="73" t="s">
+        <v>83</v>
+      </c>
+      <c r="P140" s="73"/>
+      <c r="Q140" s="73"/>
+      <c r="R140" s="73"/>
+      <c r="S140" s="73"/>
+      <c r="T140" s="73"/>
     </row>
     <row r="141" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B141" s="70"/>
@@ -9841,7 +9859,7 @@
       <c r="F142" s="13"/>
       <c r="H142" s="14">
         <f>H138+O138+O142</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I142" s="14">
         <f>I138+P138+P142</f>
@@ -9853,7 +9871,7 @@
       </c>
       <c r="K142" s="14">
         <f>K138+R138+R142</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L142" s="14">
         <f>SUM(H142:K142)</f>
@@ -9861,11 +9879,11 @@
       </c>
       <c r="M142" s="15">
         <f>(K142+I142)/L142</f>
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
       <c r="O142" s="14">
         <f>COUNTIF(L133:L134,"O")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P142" s="14">
         <f>COUNTIF(J136:J138,"N")</f>
@@ -9877,7 +9895,7 @@
       </c>
       <c r="R142" s="14">
         <f>COUNTIF(L133:L134,"R")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S142" s="14">
         <f>SUM(O142:R142)</f>
@@ -9885,13 +9903,13 @@
       </c>
       <c r="T142" s="15">
         <f>(R142+P142)/S142</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="143" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A143" s="40"/>
-      <c r="B143" s="79"/>
-      <c r="C143" s="79"/>
+      <c r="B143" s="72"/>
+      <c r="C143" s="72"/>
       <c r="D143" s="40"/>
       <c r="E143" s="40"/>
       <c r="F143" s="41"/>
@@ -9907,27 +9925,27 @@
       <c r="Q143" s="46"/>
     </row>
     <row r="144" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A144" s="73" t="s">
-        <v>114</v>
-      </c>
-      <c r="B144" s="73"/>
-      <c r="C144" s="73"/>
-      <c r="D144" s="73"/>
-      <c r="E144" s="73"/>
-      <c r="F144" s="73"/>
-      <c r="G144" s="74"/>
-      <c r="H144" s="75" t="s">
+      <c r="A144" s="74" t="s">
+        <v>113</v>
+      </c>
+      <c r="B144" s="74"/>
+      <c r="C144" s="74"/>
+      <c r="D144" s="74"/>
+      <c r="E144" s="74"/>
+      <c r="F144" s="74"/>
+      <c r="G144" s="75"/>
+      <c r="H144" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="I144" s="76"/>
-      <c r="J144" s="75" t="s">
+      <c r="I144" s="77"/>
+      <c r="J144" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="K144" s="76"/>
-      <c r="L144" s="75" t="s">
+      <c r="K144" s="77"/>
+      <c r="L144" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="M144" s="76"/>
+      <c r="M144" s="77"/>
       <c r="O144" s="52"/>
       <c r="Q144" s="52"/>
     </row>
@@ -9935,10 +9953,10 @@
       <c r="A145" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B145" s="77" t="s">
+      <c r="B145" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="C145" s="77"/>
+      <c r="C145" s="79"/>
       <c r="D145" s="55" t="s">
         <v>1</v>
       </c>
@@ -9976,18 +9994,18 @@
       <c r="A146" s="54">
         <v>23</v>
       </c>
-      <c r="B146" s="78" t="s">
-        <v>113</v>
-      </c>
-      <c r="C146" s="78"/>
+      <c r="B146" s="80" t="s">
+        <v>112</v>
+      </c>
+      <c r="C146" s="80"/>
       <c r="D146" s="50" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E146" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="F146" s="29" t="s">
         <v>117</v>
-      </c>
-      <c r="F146" s="29" t="s">
-        <v>118</v>
       </c>
       <c r="G146" s="54" t="s">
         <v>32</v>
@@ -10001,7 +10019,7 @@
       </c>
       <c r="K146" s="31"/>
       <c r="L146" s="31" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="M146" s="31"/>
       <c r="O146" s="52"/>
@@ -10011,18 +10029,18 @@
       <c r="A147" s="54">
         <v>24</v>
       </c>
-      <c r="B147" s="80" t="s">
-        <v>113</v>
-      </c>
-      <c r="C147" s="80"/>
+      <c r="B147" s="81" t="s">
+        <v>112</v>
+      </c>
+      <c r="C147" s="81"/>
       <c r="D147" s="50" t="s">
+        <v>118</v>
+      </c>
+      <c r="E147" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="F147" s="29" t="s">
         <v>119</v>
-      </c>
-      <c r="E147" s="32" t="s">
-        <v>117</v>
-      </c>
-      <c r="F147" s="29" t="s">
-        <v>120</v>
       </c>
       <c r="G147" s="54" t="s">
         <v>32</v>
@@ -10036,7 +10054,7 @@
       </c>
       <c r="K147" s="31"/>
       <c r="L147" s="31" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="M147" s="31"/>
       <c r="O147" s="52"/>
@@ -10056,22 +10074,22 @@
       <c r="B149" s="70"/>
       <c r="C149" s="70"/>
       <c r="F149" s="13"/>
-      <c r="H149" s="72" t="s">
+      <c r="H149" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="I149" s="72"/>
-      <c r="J149" s="72"/>
-      <c r="K149" s="72"/>
-      <c r="L149" s="72"/>
-      <c r="M149" s="72"/>
-      <c r="O149" s="72" t="s">
-        <v>83</v>
-      </c>
-      <c r="P149" s="72"/>
-      <c r="Q149" s="72"/>
-      <c r="R149" s="72"/>
-      <c r="S149" s="72"/>
-      <c r="T149" s="72"/>
+      <c r="I149" s="73"/>
+      <c r="J149" s="73"/>
+      <c r="K149" s="73"/>
+      <c r="L149" s="73"/>
+      <c r="M149" s="73"/>
+      <c r="O149" s="73" t="s">
+        <v>82</v>
+      </c>
+      <c r="P149" s="73"/>
+      <c r="Q149" s="73"/>
+      <c r="R149" s="73"/>
+      <c r="S149" s="73"/>
+      <c r="T149" s="73"/>
     </row>
     <row r="150" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B150" s="70"/>
@@ -10189,14 +10207,14 @@
       <c r="K153" s="71"/>
       <c r="L153" s="71"/>
       <c r="M153" s="71"/>
-      <c r="O153" s="72" t="s">
-        <v>84</v>
-      </c>
-      <c r="P153" s="72"/>
-      <c r="Q153" s="72"/>
-      <c r="R153" s="72"/>
-      <c r="S153" s="72"/>
-      <c r="T153" s="72"/>
+      <c r="O153" s="73" t="s">
+        <v>83</v>
+      </c>
+      <c r="P153" s="73"/>
+      <c r="Q153" s="73"/>
+      <c r="R153" s="73"/>
+      <c r="S153" s="73"/>
+      <c r="T153" s="73"/>
     </row>
     <row r="154" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B154" s="70"/>
@@ -10245,7 +10263,7 @@
       <c r="F155" s="13"/>
       <c r="H155" s="14">
         <f>H151+O151+O155</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I155" s="14">
         <f>I151+P151+P155</f>
@@ -10257,7 +10275,7 @@
       </c>
       <c r="K155" s="14">
         <f>K151+R151+R155</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L155" s="14">
         <f>SUM(H155:K155)</f>
@@ -10265,11 +10283,11 @@
       </c>
       <c r="M155" s="15">
         <f>(K155+I155)/L155</f>
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
       <c r="O155" s="14">
         <f>COUNTIF(L146:L147,"O")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P155" s="14">
         <f>COUNTIF(J149:J151,"N")</f>
@@ -10281,7 +10299,7 @@
       </c>
       <c r="R155" s="14">
         <f>COUNTIF(L146:L147,"R")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S155" s="14">
         <f>SUM(O155:R155)</f>
@@ -10289,13 +10307,13 @@
       </c>
       <c r="T155" s="15">
         <f>(R155+P155)/S155</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="156" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A156" s="40"/>
-      <c r="B156" s="79"/>
-      <c r="C156" s="79"/>
+      <c r="B156" s="72"/>
+      <c r="C156" s="72"/>
       <c r="D156" s="40"/>
       <c r="E156" s="40"/>
       <c r="F156" s="41"/>
@@ -10311,27 +10329,27 @@
       <c r="Q156" s="52"/>
     </row>
     <row r="157" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A157" s="73" t="s">
-        <v>116</v>
-      </c>
-      <c r="B157" s="73"/>
-      <c r="C157" s="73"/>
-      <c r="D157" s="73"/>
-      <c r="E157" s="73"/>
-      <c r="F157" s="73"/>
-      <c r="G157" s="74"/>
-      <c r="H157" s="75" t="s">
+      <c r="A157" s="74" t="s">
+        <v>115</v>
+      </c>
+      <c r="B157" s="74"/>
+      <c r="C157" s="74"/>
+      <c r="D157" s="74"/>
+      <c r="E157" s="74"/>
+      <c r="F157" s="74"/>
+      <c r="G157" s="75"/>
+      <c r="H157" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="I157" s="76"/>
-      <c r="J157" s="75" t="s">
+      <c r="I157" s="77"/>
+      <c r="J157" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="K157" s="76"/>
-      <c r="L157" s="75" t="s">
+      <c r="K157" s="77"/>
+      <c r="L157" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="M157" s="76"/>
+      <c r="M157" s="77"/>
       <c r="O157" s="52"/>
       <c r="Q157" s="52"/>
     </row>
@@ -10339,10 +10357,10 @@
       <c r="A158" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B158" s="77" t="s">
+      <c r="B158" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="C158" s="77"/>
+      <c r="C158" s="79"/>
       <c r="D158" s="55" t="s">
         <v>1</v>
       </c>
@@ -10380,18 +10398,18 @@
       <c r="A159" s="54">
         <v>25</v>
       </c>
-      <c r="B159" s="78" t="s">
-        <v>115</v>
-      </c>
-      <c r="C159" s="78"/>
+      <c r="B159" s="80" t="s">
+        <v>114</v>
+      </c>
+      <c r="C159" s="80"/>
       <c r="D159" s="50" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E159" s="32" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F159" s="29" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G159" s="54" t="s">
         <v>32</v>
@@ -10405,7 +10423,7 @@
       </c>
       <c r="K159" s="31"/>
       <c r="L159" s="31" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="M159" s="31"/>
       <c r="O159" s="52"/>
@@ -10425,28 +10443,28 @@
       <c r="B161" s="70"/>
       <c r="C161" s="70"/>
       <c r="F161" s="13"/>
-      <c r="H161" s="72" t="s">
+      <c r="H161" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="I161" s="72"/>
-      <c r="J161" s="72"/>
-      <c r="K161" s="72"/>
-      <c r="L161" s="72"/>
-      <c r="M161" s="72"/>
-      <c r="O161" s="72" t="s">
-        <v>83</v>
-      </c>
-      <c r="P161" s="72"/>
-      <c r="Q161" s="72"/>
-      <c r="R161" s="72"/>
-      <c r="S161" s="72"/>
-      <c r="T161" s="72"/>
+      <c r="I161" s="73"/>
+      <c r="J161" s="73"/>
+      <c r="K161" s="73"/>
+      <c r="L161" s="73"/>
+      <c r="M161" s="73"/>
+      <c r="O161" s="73" t="s">
+        <v>82</v>
+      </c>
+      <c r="P161" s="73"/>
+      <c r="Q161" s="73"/>
+      <c r="R161" s="73"/>
+      <c r="S161" s="73"/>
+      <c r="T161" s="73"/>
     </row>
     <row r="162" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B162" s="70"/>
       <c r="C162" s="70"/>
       <c r="E162" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F162" s="13"/>
       <c r="H162" s="16" t="s">
@@ -10561,14 +10579,14 @@
       <c r="K165" s="71"/>
       <c r="L165" s="71"/>
       <c r="M165" s="71"/>
-      <c r="O165" s="72" t="s">
-        <v>84</v>
-      </c>
-      <c r="P165" s="72"/>
-      <c r="Q165" s="72"/>
-      <c r="R165" s="72"/>
-      <c r="S165" s="72"/>
-      <c r="T165" s="72"/>
+      <c r="O165" s="73" t="s">
+        <v>83</v>
+      </c>
+      <c r="P165" s="73"/>
+      <c r="Q165" s="73"/>
+      <c r="R165" s="73"/>
+      <c r="S165" s="73"/>
+      <c r="T165" s="73"/>
     </row>
     <row r="166" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B166" s="70"/>
@@ -10617,7 +10635,7 @@
       <c r="F167" s="13"/>
       <c r="H167" s="14">
         <f>H163+O163+O167</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I167" s="14">
         <f>I163+P163+P167</f>
@@ -10629,7 +10647,7 @@
       </c>
       <c r="K167" s="14">
         <f>K163+R163+R167</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L167" s="14">
         <f>SUM(H167:K167)</f>
@@ -10637,11 +10655,11 @@
       </c>
       <c r="M167" s="15">
         <f>(K167+I167)/L167</f>
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
       <c r="O167" s="14">
         <f>COUNTIF(L159:L159,"O")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P167" s="14">
         <f>COUNTIF(J161:J163,"N")</f>
@@ -10653,7 +10671,7 @@
       </c>
       <c r="R167" s="14">
         <f>COUNTIF(L159:L159,"R")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S167" s="14">
         <f>SUM(O167:R167)</f>
@@ -10661,13 +10679,13 @@
       </c>
       <c r="T167" s="15">
         <f>(R167+P167)/S167</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="168" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A168" s="40"/>
-      <c r="B168" s="79"/>
-      <c r="C168" s="79"/>
+      <c r="B168" s="72"/>
+      <c r="C168" s="72"/>
       <c r="D168" s="40"/>
       <c r="E168" s="40"/>
       <c r="F168" s="41"/>
@@ -10683,27 +10701,27 @@
       <c r="Q168" s="52"/>
     </row>
     <row r="169" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A169" s="73" t="s">
-        <v>131</v>
-      </c>
-      <c r="B169" s="73"/>
-      <c r="C169" s="73"/>
-      <c r="D169" s="73"/>
-      <c r="E169" s="73"/>
-      <c r="F169" s="73"/>
-      <c r="G169" s="74"/>
-      <c r="H169" s="75" t="s">
+      <c r="A169" s="74" t="s">
+        <v>130</v>
+      </c>
+      <c r="B169" s="74"/>
+      <c r="C169" s="74"/>
+      <c r="D169" s="74"/>
+      <c r="E169" s="74"/>
+      <c r="F169" s="74"/>
+      <c r="G169" s="75"/>
+      <c r="H169" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="I169" s="76"/>
-      <c r="J169" s="75" t="s">
+      <c r="I169" s="77"/>
+      <c r="J169" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="K169" s="76"/>
-      <c r="L169" s="75" t="s">
+      <c r="K169" s="77"/>
+      <c r="L169" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="M169" s="76"/>
+      <c r="M169" s="77"/>
       <c r="O169" s="56"/>
       <c r="Q169" s="56"/>
     </row>
@@ -10711,10 +10729,10 @@
       <c r="A170" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="B170" s="77" t="s">
+      <c r="B170" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="C170" s="77"/>
+      <c r="C170" s="79"/>
       <c r="D170" s="60" t="s">
         <v>1</v>
       </c>
@@ -10752,18 +10770,18 @@
       <c r="A171" s="58">
         <v>26</v>
       </c>
-      <c r="B171" s="78" t="s">
-        <v>132</v>
-      </c>
-      <c r="C171" s="78"/>
+      <c r="B171" s="80" t="s">
+        <v>131</v>
+      </c>
+      <c r="C171" s="80"/>
       <c r="D171" s="50" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E171" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="F171" s="29" t="s">
         <v>154</v>
-      </c>
-      <c r="F171" s="29" t="s">
-        <v>155</v>
       </c>
       <c r="G171" s="58" t="s">
         <v>32</v>
@@ -10777,7 +10795,7 @@
       </c>
       <c r="K171" s="31"/>
       <c r="L171" s="31" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="M171" s="31"/>
       <c r="O171" s="56"/>
@@ -10797,22 +10815,22 @@
       <c r="B173" s="70"/>
       <c r="C173" s="70"/>
       <c r="F173" s="13"/>
-      <c r="H173" s="72" t="s">
+      <c r="H173" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="I173" s="72"/>
-      <c r="J173" s="72"/>
-      <c r="K173" s="72"/>
-      <c r="L173" s="72"/>
-      <c r="M173" s="72"/>
-      <c r="O173" s="72" t="s">
-        <v>83</v>
-      </c>
-      <c r="P173" s="72"/>
-      <c r="Q173" s="72"/>
-      <c r="R173" s="72"/>
-      <c r="S173" s="72"/>
-      <c r="T173" s="72"/>
+      <c r="I173" s="73"/>
+      <c r="J173" s="73"/>
+      <c r="K173" s="73"/>
+      <c r="L173" s="73"/>
+      <c r="M173" s="73"/>
+      <c r="O173" s="73" t="s">
+        <v>82</v>
+      </c>
+      <c r="P173" s="73"/>
+      <c r="Q173" s="73"/>
+      <c r="R173" s="73"/>
+      <c r="S173" s="73"/>
+      <c r="T173" s="73"/>
     </row>
     <row r="174" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B174" s="70"/>
@@ -10930,14 +10948,14 @@
       <c r="K177" s="71"/>
       <c r="L177" s="71"/>
       <c r="M177" s="71"/>
-      <c r="O177" s="72" t="s">
-        <v>84</v>
-      </c>
-      <c r="P177" s="72"/>
-      <c r="Q177" s="72"/>
-      <c r="R177" s="72"/>
-      <c r="S177" s="72"/>
-      <c r="T177" s="72"/>
+      <c r="O177" s="73" t="s">
+        <v>83</v>
+      </c>
+      <c r="P177" s="73"/>
+      <c r="Q177" s="73"/>
+      <c r="R177" s="73"/>
+      <c r="S177" s="73"/>
+      <c r="T177" s="73"/>
     </row>
     <row r="178" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B178" s="70"/>
@@ -10986,7 +11004,7 @@
       <c r="F179" s="13"/>
       <c r="H179" s="14">
         <f>H175+O175+O179</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I179" s="14">
         <f>I175+P175+P179</f>
@@ -10998,7 +11016,7 @@
       </c>
       <c r="K179" s="14">
         <f>K175+R175+R179</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L179" s="14">
         <f>SUM(H179:K179)</f>
@@ -11006,11 +11024,11 @@
       </c>
       <c r="M179" s="15">
         <f>(K179+I179)/L179</f>
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
       <c r="O179" s="14">
         <f>COUNTIF(L171:L171,"O")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P179" s="14">
         <f>COUNTIF(J173:J175,"N")</f>
@@ -11022,7 +11040,7 @@
       </c>
       <c r="R179" s="14">
         <f>COUNTIF(L171:L171,"R")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S179" s="14">
         <f>SUM(O179:R179)</f>
@@ -11030,13 +11048,13 @@
       </c>
       <c r="T179" s="15">
         <f>(R179+P179)/S179</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="180" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A180" s="40"/>
-      <c r="B180" s="79"/>
-      <c r="C180" s="79"/>
+      <c r="B180" s="72"/>
+      <c r="C180" s="72"/>
       <c r="D180" s="40"/>
       <c r="E180" s="40"/>
       <c r="F180" s="41"/>
@@ -11052,27 +11070,27 @@
       <c r="Q180" s="56"/>
     </row>
     <row r="181" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A181" s="73" t="s">
+      <c r="A181" s="74" t="s">
         <v>63</v>
       </c>
-      <c r="B181" s="73"/>
-      <c r="C181" s="73"/>
-      <c r="D181" s="73"/>
-      <c r="E181" s="73"/>
-      <c r="F181" s="73"/>
-      <c r="G181" s="74"/>
-      <c r="H181" s="75" t="s">
+      <c r="B181" s="74"/>
+      <c r="C181" s="74"/>
+      <c r="D181" s="74"/>
+      <c r="E181" s="74"/>
+      <c r="F181" s="74"/>
+      <c r="G181" s="75"/>
+      <c r="H181" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="I181" s="76"/>
-      <c r="J181" s="75" t="s">
+      <c r="I181" s="77"/>
+      <c r="J181" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="K181" s="76"/>
-      <c r="L181" s="75" t="s">
+      <c r="K181" s="77"/>
+      <c r="L181" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="M181" s="76"/>
+      <c r="M181" s="77"/>
       <c r="O181" s="37"/>
       <c r="Q181" s="37"/>
     </row>
@@ -11080,10 +11098,10 @@
       <c r="A182" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B182" s="77" t="s">
+      <c r="B182" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="C182" s="77"/>
+      <c r="C182" s="79"/>
       <c r="D182" s="38" t="s">
         <v>1</v>
       </c>
@@ -11121,10 +11139,10 @@
       <c r="A183" s="39">
         <v>27</v>
       </c>
-      <c r="B183" s="78" t="s">
+      <c r="B183" s="80" t="s">
         <v>64</v>
       </c>
-      <c r="C183" s="78"/>
+      <c r="C183" s="80"/>
       <c r="D183" s="34" t="s">
         <v>64</v>
       </c>
@@ -11146,7 +11164,7 @@
       </c>
       <c r="K183" s="31"/>
       <c r="L183" s="31" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="M183" s="31"/>
       <c r="O183" s="37"/>
@@ -11156,10 +11174,10 @@
       <c r="A184" s="39">
         <v>28</v>
       </c>
-      <c r="B184" s="80" t="s">
+      <c r="B184" s="81" t="s">
         <v>64</v>
       </c>
-      <c r="C184" s="80"/>
+      <c r="C184" s="81"/>
       <c r="D184" s="34" t="s">
         <v>68</v>
       </c>
@@ -11181,7 +11199,7 @@
       </c>
       <c r="K184" s="31"/>
       <c r="L184" s="31" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="M184" s="31"/>
       <c r="O184" s="37"/>
@@ -11191,10 +11209,10 @@
       <c r="A185" s="68">
         <v>29</v>
       </c>
-      <c r="B185" s="69" t="s">
+      <c r="B185" s="78" t="s">
         <v>64</v>
       </c>
-      <c r="C185" s="69"/>
+      <c r="C185" s="78"/>
       <c r="D185" s="34" t="s">
         <v>68</v>
       </c>
@@ -11216,7 +11234,7 @@
       </c>
       <c r="K185" s="31"/>
       <c r="L185" s="31" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="M185" s="31"/>
       <c r="O185" s="37"/>
@@ -11226,10 +11244,10 @@
       <c r="A186" s="68">
         <v>30</v>
       </c>
-      <c r="B186" s="69" t="s">
+      <c r="B186" s="78" t="s">
         <v>64</v>
       </c>
-      <c r="C186" s="69"/>
+      <c r="C186" s="78"/>
       <c r="D186" s="34" t="s">
         <v>68</v>
       </c>
@@ -11251,7 +11269,7 @@
       </c>
       <c r="K186" s="31"/>
       <c r="L186" s="31" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="M186" s="31"/>
       <c r="O186" s="43"/>
@@ -11261,10 +11279,10 @@
       <c r="A187" s="68">
         <v>31</v>
       </c>
-      <c r="B187" s="69" t="s">
+      <c r="B187" s="78" t="s">
         <v>64</v>
       </c>
-      <c r="C187" s="69"/>
+      <c r="C187" s="78"/>
       <c r="D187" s="34" t="s">
         <v>68</v>
       </c>
@@ -11286,7 +11304,7 @@
       </c>
       <c r="K187" s="31"/>
       <c r="L187" s="31" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="M187" s="31"/>
       <c r="O187" s="43"/>
@@ -11296,10 +11314,10 @@
       <c r="A188" s="68">
         <v>32</v>
       </c>
-      <c r="B188" s="69" t="s">
+      <c r="B188" s="78" t="s">
         <v>64</v>
       </c>
-      <c r="C188" s="69"/>
+      <c r="C188" s="78"/>
       <c r="D188" s="34" t="s">
         <v>68</v>
       </c>
@@ -11321,7 +11339,7 @@
       </c>
       <c r="K188" s="31"/>
       <c r="L188" s="31" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="M188" s="31"/>
       <c r="O188" s="43"/>
@@ -11331,10 +11349,10 @@
       <c r="A189" s="68">
         <v>33</v>
       </c>
-      <c r="B189" s="69" t="s">
+      <c r="B189" s="78" t="s">
         <v>64</v>
       </c>
-      <c r="C189" s="69"/>
+      <c r="C189" s="78"/>
       <c r="D189" s="34" t="s">
         <v>78</v>
       </c>
@@ -11356,7 +11374,7 @@
       </c>
       <c r="K189" s="31"/>
       <c r="L189" s="31" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="M189" s="31"/>
       <c r="O189" s="43"/>
@@ -11366,18 +11384,18 @@
       <c r="A190" s="68">
         <v>34</v>
       </c>
-      <c r="B190" s="69" t="s">
+      <c r="B190" s="78" t="s">
         <v>64</v>
       </c>
-      <c r="C190" s="69"/>
+      <c r="C190" s="78"/>
       <c r="D190" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="E190" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="E190" s="32" t="s">
+      <c r="F190" s="29" t="s">
         <v>101</v>
-      </c>
-      <c r="F190" s="29" t="s">
-        <v>102</v>
       </c>
       <c r="G190" s="44" t="s">
         <v>32</v>
@@ -11391,7 +11409,7 @@
       </c>
       <c r="K190" s="31"/>
       <c r="L190" s="31" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="M190" s="31"/>
       <c r="O190" s="43"/>
@@ -11411,22 +11429,22 @@
       <c r="B192" s="70"/>
       <c r="C192" s="70"/>
       <c r="F192" s="13"/>
-      <c r="H192" s="72" t="s">
+      <c r="H192" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="I192" s="72"/>
-      <c r="J192" s="72"/>
-      <c r="K192" s="72"/>
-      <c r="L192" s="72"/>
-      <c r="M192" s="72"/>
-      <c r="O192" s="72" t="s">
-        <v>83</v>
-      </c>
-      <c r="P192" s="72"/>
-      <c r="Q192" s="72"/>
-      <c r="R192" s="72"/>
-      <c r="S192" s="72"/>
-      <c r="T192" s="72"/>
+      <c r="I192" s="73"/>
+      <c r="J192" s="73"/>
+      <c r="K192" s="73"/>
+      <c r="L192" s="73"/>
+      <c r="M192" s="73"/>
+      <c r="O192" s="73" t="s">
+        <v>82</v>
+      </c>
+      <c r="P192" s="73"/>
+      <c r="Q192" s="73"/>
+      <c r="R192" s="73"/>
+      <c r="S192" s="73"/>
+      <c r="T192" s="73"/>
     </row>
     <row r="193" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B193" s="70"/>
@@ -11544,14 +11562,14 @@
       <c r="K196" s="71"/>
       <c r="L196" s="71"/>
       <c r="M196" s="71"/>
-      <c r="O196" s="72" t="s">
-        <v>84</v>
-      </c>
-      <c r="P196" s="72"/>
-      <c r="Q196" s="72"/>
-      <c r="R196" s="72"/>
-      <c r="S196" s="72"/>
-      <c r="T196" s="72"/>
+      <c r="O196" s="73" t="s">
+        <v>83</v>
+      </c>
+      <c r="P196" s="73"/>
+      <c r="Q196" s="73"/>
+      <c r="R196" s="73"/>
+      <c r="S196" s="73"/>
+      <c r="T196" s="73"/>
     </row>
     <row r="197" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B197" s="70"/>
@@ -11600,7 +11618,7 @@
       <c r="F198" s="13"/>
       <c r="H198" s="14">
         <f>H194+O194+O198</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="I198" s="14">
         <f>I194+P194+P198</f>
@@ -11612,7 +11630,7 @@
       </c>
       <c r="K198" s="14">
         <f>K194+R194+R198</f>
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="L198" s="14">
         <f>SUM(H198:K198)</f>
@@ -11620,11 +11638,11 @@
       </c>
       <c r="M198" s="15">
         <f>(K198+I198)/L198</f>
-        <v>0.60869565217391308</v>
+        <v>0.95652173913043481</v>
       </c>
       <c r="O198" s="14">
         <f>COUNTIF(L183:L190,"O")</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="P198" s="14">
         <f>COUNTIF(J192:J194,"N")</f>
@@ -11636,7 +11654,7 @@
       </c>
       <c r="R198" s="14">
         <f>COUNTIF(L183:L190,"R")</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="S198" s="14">
         <f>SUM(O198:R198)</f>
@@ -11644,13 +11662,13 @@
       </c>
       <c r="T198" s="15">
         <f>(R198+P198)/S198</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="199" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A199" s="40"/>
-      <c r="B199" s="79"/>
-      <c r="C199" s="79"/>
+      <c r="B199" s="72"/>
+      <c r="C199" s="72"/>
       <c r="D199" s="40"/>
       <c r="E199" s="40"/>
       <c r="F199" s="41"/>
@@ -11667,16 +11685,260 @@
     </row>
   </sheetData>
   <mergeCells count="288">
-    <mergeCell ref="B196:C196"/>
-    <mergeCell ref="H196:M196"/>
-    <mergeCell ref="B197:C197"/>
-    <mergeCell ref="B198:C198"/>
-    <mergeCell ref="B199:C199"/>
-    <mergeCell ref="B192:C192"/>
-    <mergeCell ref="H192:M192"/>
-    <mergeCell ref="B193:C193"/>
-    <mergeCell ref="B194:C194"/>
-    <mergeCell ref="B195:C195"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B124:C124"/>
+    <mergeCell ref="B125:C125"/>
+    <mergeCell ref="B126:C126"/>
+    <mergeCell ref="B127:C127"/>
+    <mergeCell ref="H127:M127"/>
+    <mergeCell ref="O127:T127"/>
+    <mergeCell ref="B128:C128"/>
+    <mergeCell ref="B129:C129"/>
+    <mergeCell ref="A119:G119"/>
+    <mergeCell ref="H119:I119"/>
+    <mergeCell ref="J119:K119"/>
+    <mergeCell ref="L119:M119"/>
+    <mergeCell ref="B120:C120"/>
+    <mergeCell ref="B121:C121"/>
+    <mergeCell ref="B122:C122"/>
+    <mergeCell ref="B123:C123"/>
+    <mergeCell ref="H123:M123"/>
+    <mergeCell ref="O89:T89"/>
+    <mergeCell ref="O98:T98"/>
+    <mergeCell ref="O102:T102"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B166:C166"/>
+    <mergeCell ref="B167:C167"/>
+    <mergeCell ref="B168:C168"/>
+    <mergeCell ref="B160:C160"/>
+    <mergeCell ref="B161:C161"/>
+    <mergeCell ref="H161:M161"/>
+    <mergeCell ref="O161:T161"/>
+    <mergeCell ref="B162:C162"/>
+    <mergeCell ref="B163:C163"/>
+    <mergeCell ref="B164:C164"/>
+    <mergeCell ref="B165:C165"/>
+    <mergeCell ref="H165:M165"/>
+    <mergeCell ref="O165:T165"/>
+    <mergeCell ref="B155:C155"/>
+    <mergeCell ref="B156:C156"/>
+    <mergeCell ref="A157:G157"/>
+    <mergeCell ref="H157:I157"/>
+    <mergeCell ref="J157:K157"/>
+    <mergeCell ref="L157:M157"/>
+    <mergeCell ref="B158:C158"/>
+    <mergeCell ref="B159:C159"/>
+    <mergeCell ref="B151:C151"/>
+    <mergeCell ref="B152:C152"/>
+    <mergeCell ref="B153:C153"/>
+    <mergeCell ref="B154:C154"/>
+    <mergeCell ref="A144:G144"/>
+    <mergeCell ref="H144:I144"/>
+    <mergeCell ref="J144:K144"/>
+    <mergeCell ref="L144:M144"/>
+    <mergeCell ref="H149:M149"/>
+    <mergeCell ref="O149:T149"/>
+    <mergeCell ref="H153:M153"/>
+    <mergeCell ref="O153:T153"/>
+    <mergeCell ref="B145:C145"/>
+    <mergeCell ref="B146:C146"/>
+    <mergeCell ref="B147:C147"/>
+    <mergeCell ref="B148:C148"/>
+    <mergeCell ref="B149:C149"/>
+    <mergeCell ref="B150:C150"/>
+    <mergeCell ref="B137:C137"/>
+    <mergeCell ref="B138:C138"/>
+    <mergeCell ref="B139:C139"/>
+    <mergeCell ref="B140:C140"/>
+    <mergeCell ref="H140:M140"/>
+    <mergeCell ref="O140:T140"/>
+    <mergeCell ref="B141:C141"/>
+    <mergeCell ref="B142:C142"/>
+    <mergeCell ref="A131:G131"/>
+    <mergeCell ref="H131:I131"/>
+    <mergeCell ref="J131:K131"/>
+    <mergeCell ref="L131:M131"/>
+    <mergeCell ref="B132:C132"/>
+    <mergeCell ref="B133:C133"/>
+    <mergeCell ref="B134:C134"/>
+    <mergeCell ref="B135:C135"/>
+    <mergeCell ref="B136:C136"/>
+    <mergeCell ref="H136:M136"/>
+    <mergeCell ref="O192:T192"/>
+    <mergeCell ref="O196:T196"/>
+    <mergeCell ref="O48:T48"/>
+    <mergeCell ref="O52:T52"/>
+    <mergeCell ref="O111:T111"/>
+    <mergeCell ref="O115:T115"/>
+    <mergeCell ref="O136:T136"/>
+    <mergeCell ref="O173:T173"/>
+    <mergeCell ref="O177:T177"/>
+    <mergeCell ref="O123:T123"/>
+    <mergeCell ref="O16:T16"/>
+    <mergeCell ref="O20:T20"/>
+    <mergeCell ref="O33:T33"/>
+    <mergeCell ref="O37:T37"/>
+    <mergeCell ref="O61:T61"/>
+    <mergeCell ref="O65:T65"/>
+    <mergeCell ref="O73:T73"/>
+    <mergeCell ref="O77:T77"/>
+    <mergeCell ref="O85:T85"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="H65:M65"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="A56:G56"/>
+    <mergeCell ref="H56:I56"/>
+    <mergeCell ref="J56:K56"/>
+    <mergeCell ref="L56:M56"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="H61:M61"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="H48:M48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="H52:M52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="A41:G41"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="H16:M16"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H20:M20"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="A69:G69"/>
+    <mergeCell ref="H69:I69"/>
+    <mergeCell ref="J69:K69"/>
+    <mergeCell ref="L69:M69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="H33:M33"/>
+    <mergeCell ref="H37:M37"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="L41:M41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="H73:M73"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="H77:M77"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="J81:K81"/>
+    <mergeCell ref="L81:M81"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="A81:G81"/>
+    <mergeCell ref="H81:I81"/>
+    <mergeCell ref="B87:C87"/>
+    <mergeCell ref="B88:C88"/>
+    <mergeCell ref="B89:C89"/>
+    <mergeCell ref="H89:M89"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="H85:M85"/>
+    <mergeCell ref="B86:C86"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="B108:C108"/>
+    <mergeCell ref="B109:C109"/>
+    <mergeCell ref="B110:C110"/>
+    <mergeCell ref="B111:C111"/>
+    <mergeCell ref="H111:M111"/>
+    <mergeCell ref="B112:C112"/>
+    <mergeCell ref="B101:C101"/>
+    <mergeCell ref="B102:C102"/>
+    <mergeCell ref="H102:M102"/>
+    <mergeCell ref="B103:C103"/>
+    <mergeCell ref="B104:C104"/>
+    <mergeCell ref="L93:M93"/>
+    <mergeCell ref="B94:C94"/>
+    <mergeCell ref="B95:C95"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="B91:C91"/>
+    <mergeCell ref="B92:C92"/>
+    <mergeCell ref="A93:G93"/>
+    <mergeCell ref="H93:I93"/>
+    <mergeCell ref="J93:K93"/>
+    <mergeCell ref="B97:C97"/>
+    <mergeCell ref="B98:C98"/>
+    <mergeCell ref="H98:M98"/>
+    <mergeCell ref="B99:C99"/>
+    <mergeCell ref="B100:C100"/>
+    <mergeCell ref="B182:C182"/>
+    <mergeCell ref="B183:C183"/>
+    <mergeCell ref="B184:C184"/>
+    <mergeCell ref="B185:C185"/>
+    <mergeCell ref="B171:C171"/>
+    <mergeCell ref="B172:C172"/>
+    <mergeCell ref="B173:C173"/>
+    <mergeCell ref="H173:M173"/>
+    <mergeCell ref="B174:C174"/>
+    <mergeCell ref="B175:C175"/>
+    <mergeCell ref="B176:C176"/>
+    <mergeCell ref="B177:C177"/>
+    <mergeCell ref="H177:M177"/>
+    <mergeCell ref="B178:C178"/>
+    <mergeCell ref="B179:C179"/>
+    <mergeCell ref="B180:C180"/>
+    <mergeCell ref="B113:C113"/>
+    <mergeCell ref="J106:K106"/>
+    <mergeCell ref="L106:M106"/>
     <mergeCell ref="B191:C191"/>
     <mergeCell ref="B105:C105"/>
     <mergeCell ref="A181:G181"/>
@@ -11701,260 +11963,16 @@
     <mergeCell ref="J169:K169"/>
     <mergeCell ref="L169:M169"/>
     <mergeCell ref="B170:C170"/>
-    <mergeCell ref="B97:C97"/>
-    <mergeCell ref="B98:C98"/>
-    <mergeCell ref="H98:M98"/>
-    <mergeCell ref="B99:C99"/>
-    <mergeCell ref="B100:C100"/>
-    <mergeCell ref="B182:C182"/>
-    <mergeCell ref="B183:C183"/>
-    <mergeCell ref="B184:C184"/>
-    <mergeCell ref="B185:C185"/>
-    <mergeCell ref="B171:C171"/>
-    <mergeCell ref="B172:C172"/>
-    <mergeCell ref="B173:C173"/>
-    <mergeCell ref="H173:M173"/>
-    <mergeCell ref="B174:C174"/>
-    <mergeCell ref="B175:C175"/>
-    <mergeCell ref="B176:C176"/>
-    <mergeCell ref="B177:C177"/>
-    <mergeCell ref="H177:M177"/>
-    <mergeCell ref="B178:C178"/>
-    <mergeCell ref="B179:C179"/>
-    <mergeCell ref="B180:C180"/>
-    <mergeCell ref="B113:C113"/>
-    <mergeCell ref="J106:K106"/>
-    <mergeCell ref="L106:M106"/>
-    <mergeCell ref="L93:M93"/>
-    <mergeCell ref="B94:C94"/>
-    <mergeCell ref="B95:C95"/>
-    <mergeCell ref="B96:C96"/>
-    <mergeCell ref="B91:C91"/>
-    <mergeCell ref="B92:C92"/>
-    <mergeCell ref="A93:G93"/>
-    <mergeCell ref="H93:I93"/>
-    <mergeCell ref="J93:K93"/>
-    <mergeCell ref="B107:C107"/>
-    <mergeCell ref="B108:C108"/>
-    <mergeCell ref="B109:C109"/>
-    <mergeCell ref="B110:C110"/>
-    <mergeCell ref="B111:C111"/>
-    <mergeCell ref="H111:M111"/>
-    <mergeCell ref="B112:C112"/>
-    <mergeCell ref="B101:C101"/>
-    <mergeCell ref="B102:C102"/>
-    <mergeCell ref="H102:M102"/>
-    <mergeCell ref="B103:C103"/>
-    <mergeCell ref="B104:C104"/>
-    <mergeCell ref="B87:C87"/>
-    <mergeCell ref="B88:C88"/>
-    <mergeCell ref="B89:C89"/>
-    <mergeCell ref="H89:M89"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="H85:M85"/>
-    <mergeCell ref="B86:C86"/>
-    <mergeCell ref="J81:K81"/>
-    <mergeCell ref="L81:M81"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="A81:G81"/>
-    <mergeCell ref="H81:I81"/>
-    <mergeCell ref="H73:M73"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="H77:M77"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="A69:G69"/>
-    <mergeCell ref="H69:I69"/>
-    <mergeCell ref="J69:K69"/>
-    <mergeCell ref="L69:M69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="H33:M33"/>
-    <mergeCell ref="H37:M37"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="J41:K41"/>
-    <mergeCell ref="L41:M41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="H20:M20"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="A10:G10"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="H16:M16"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="A41:G41"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="A25:G25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="H48:M48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="H52:M52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="H65:M65"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="A56:G56"/>
-    <mergeCell ref="H56:I56"/>
-    <mergeCell ref="J56:K56"/>
-    <mergeCell ref="L56:M56"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="H61:M61"/>
-    <mergeCell ref="O16:T16"/>
-    <mergeCell ref="O20:T20"/>
-    <mergeCell ref="O33:T33"/>
-    <mergeCell ref="O37:T37"/>
-    <mergeCell ref="O61:T61"/>
-    <mergeCell ref="O65:T65"/>
-    <mergeCell ref="O73:T73"/>
-    <mergeCell ref="O77:T77"/>
-    <mergeCell ref="O85:T85"/>
-    <mergeCell ref="O192:T192"/>
-    <mergeCell ref="O196:T196"/>
-    <mergeCell ref="O48:T48"/>
-    <mergeCell ref="O52:T52"/>
-    <mergeCell ref="O111:T111"/>
-    <mergeCell ref="O115:T115"/>
-    <mergeCell ref="O136:T136"/>
-    <mergeCell ref="O173:T173"/>
-    <mergeCell ref="O177:T177"/>
-    <mergeCell ref="O123:T123"/>
-    <mergeCell ref="B137:C137"/>
-    <mergeCell ref="B138:C138"/>
-    <mergeCell ref="B139:C139"/>
-    <mergeCell ref="B140:C140"/>
-    <mergeCell ref="H140:M140"/>
-    <mergeCell ref="O140:T140"/>
-    <mergeCell ref="B141:C141"/>
-    <mergeCell ref="B142:C142"/>
-    <mergeCell ref="A131:G131"/>
-    <mergeCell ref="H131:I131"/>
-    <mergeCell ref="J131:K131"/>
-    <mergeCell ref="L131:M131"/>
-    <mergeCell ref="B132:C132"/>
-    <mergeCell ref="B133:C133"/>
-    <mergeCell ref="B134:C134"/>
-    <mergeCell ref="B135:C135"/>
-    <mergeCell ref="B136:C136"/>
-    <mergeCell ref="H136:M136"/>
-    <mergeCell ref="A144:G144"/>
-    <mergeCell ref="H144:I144"/>
-    <mergeCell ref="J144:K144"/>
-    <mergeCell ref="L144:M144"/>
-    <mergeCell ref="H149:M149"/>
-    <mergeCell ref="O149:T149"/>
-    <mergeCell ref="H153:M153"/>
-    <mergeCell ref="O153:T153"/>
-    <mergeCell ref="B145:C145"/>
-    <mergeCell ref="B146:C146"/>
-    <mergeCell ref="B147:C147"/>
-    <mergeCell ref="B148:C148"/>
-    <mergeCell ref="B149:C149"/>
-    <mergeCell ref="B150:C150"/>
-    <mergeCell ref="B155:C155"/>
-    <mergeCell ref="B156:C156"/>
-    <mergeCell ref="A157:G157"/>
-    <mergeCell ref="H157:I157"/>
-    <mergeCell ref="J157:K157"/>
-    <mergeCell ref="L157:M157"/>
-    <mergeCell ref="B158:C158"/>
-    <mergeCell ref="B159:C159"/>
-    <mergeCell ref="B151:C151"/>
-    <mergeCell ref="B152:C152"/>
-    <mergeCell ref="B153:C153"/>
-    <mergeCell ref="B154:C154"/>
-    <mergeCell ref="B166:C166"/>
-    <mergeCell ref="B167:C167"/>
-    <mergeCell ref="B168:C168"/>
-    <mergeCell ref="B160:C160"/>
-    <mergeCell ref="B161:C161"/>
-    <mergeCell ref="H161:M161"/>
-    <mergeCell ref="O161:T161"/>
-    <mergeCell ref="B162:C162"/>
-    <mergeCell ref="B163:C163"/>
-    <mergeCell ref="B164:C164"/>
-    <mergeCell ref="B165:C165"/>
-    <mergeCell ref="H165:M165"/>
-    <mergeCell ref="O165:T165"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B124:C124"/>
-    <mergeCell ref="B125:C125"/>
-    <mergeCell ref="B126:C126"/>
-    <mergeCell ref="B127:C127"/>
-    <mergeCell ref="H127:M127"/>
-    <mergeCell ref="O127:T127"/>
-    <mergeCell ref="B128:C128"/>
-    <mergeCell ref="B129:C129"/>
-    <mergeCell ref="A119:G119"/>
-    <mergeCell ref="H119:I119"/>
-    <mergeCell ref="J119:K119"/>
-    <mergeCell ref="L119:M119"/>
-    <mergeCell ref="B120:C120"/>
-    <mergeCell ref="B121:C121"/>
-    <mergeCell ref="B122:C122"/>
-    <mergeCell ref="B123:C123"/>
-    <mergeCell ref="H123:M123"/>
-    <mergeCell ref="O89:T89"/>
-    <mergeCell ref="O98:T98"/>
-    <mergeCell ref="O102:T102"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B196:C196"/>
+    <mergeCell ref="H196:M196"/>
+    <mergeCell ref="B197:C197"/>
+    <mergeCell ref="B198:C198"/>
+    <mergeCell ref="B199:C199"/>
+    <mergeCell ref="B192:C192"/>
+    <mergeCell ref="H192:M192"/>
+    <mergeCell ref="B193:C193"/>
+    <mergeCell ref="B194:C194"/>
+    <mergeCell ref="B195:C195"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:B9">
     <cfRule type="colorScale" priority="1143">

</xml_diff>

<commit_message>
Updated List of TestCases
</commit_message>
<xml_diff>
--- a/Basisverzeichnis/trunk/04_Test/Systemtest_TestCases.xlsx
+++ b/Basisverzeichnis/trunk/04_Test/Systemtest_TestCases.xlsx
@@ -164,9 +164,6 @@
 2. Der Anwender wählt den Pfad zu seinem UseCaseDokument
 3. Der Anwender wählt sein Dokument aus und bestätigt den Dialog mit dem Button "Öffnen"
 4. Das Tool gibt dem Anwender Feedback darüber, dass das Word-Dokument nicht eingelesen werden kann. Das Tool informiert über die Ursache des Fehlers (Kann WORD-Dokument nicht öffnen, Fehler in der Dokumentstruktur, leeres Dokument)</t>
-  </si>
-  <si>
-    <t>Das einzulesende UseCase-Dokument ist ein leeres WORD-Dokuement</t>
   </si>
   <si>
     <t>Das UseCase-Dokument ist leer (Tool soll melden, dass die Datei leer ist)</t>
@@ -630,7 +627,11 @@
     <t>Anpassungen der Darstellungen waren notwendig aufgrund Funktionalitätsänderung (Ende - Knoten entfernt)</t>
   </si>
   <si>
-    <t>Dritter Testdurchlauf am 29.06.2015</t>
+    <t>Das einzulesende UseCase-Dokument ist ein leeres WORD-Dokuement
+(TestFile: UseCase_Empty.docx)</t>
+  </si>
+  <si>
+    <t>Dritter Testdurchlauf am 29.06.2015 + 30.06.2015</t>
   </si>
 </sst>
 </file>
@@ -1135,12 +1136,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
@@ -1158,20 +1159,20 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1179,8 +1180,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -5665,8 +5666,8 @@
   </sheetPr>
   <dimension ref="A1:T199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5701,15 +5702,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
-      <c r="G1" s="85"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
       <c r="H1" s="12"/>
       <c r="I1" s="7"/>
       <c r="J1" s="12"/>
@@ -5723,15 +5724,15 @@
       <c r="R1" s="7"/>
     </row>
     <row r="2" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="82" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="85"/>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
+      <c r="B2" s="82"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
       <c r="H2" s="12"/>
       <c r="I2" s="7"/>
       <c r="J2" s="12"/>
@@ -5762,7 +5763,7 @@
       <c r="D4" s="19"/>
       <c r="E4" s="22"/>
       <c r="F4" s="22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -5776,7 +5777,7 @@
       <c r="D5" s="19"/>
       <c r="E5" s="22"/>
       <c r="F5" s="22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H5"/>
       <c r="J5"/>
@@ -5817,7 +5818,7 @@
       </c>
       <c r="D8" s="19"/>
       <c r="E8" s="22" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F8" s="22"/>
     </row>
@@ -5902,7 +5903,7 @@
       </c>
       <c r="C12" s="84"/>
       <c r="D12" s="34" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E12" s="32" t="s">
         <v>31</v>
@@ -5934,12 +5935,12 @@
       <c r="A13" s="35">
         <v>2</v>
       </c>
-      <c r="B13" s="78" t="s">
+      <c r="B13" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="78"/>
+      <c r="C13" s="70"/>
       <c r="D13" s="34" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E13" s="32" t="s">
         <v>37</v>
@@ -5969,12 +5970,12 @@
       <c r="A14" s="30">
         <v>3</v>
       </c>
-      <c r="B14" s="78" t="s">
+      <c r="B14" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="78"/>
+      <c r="C14" s="70"/>
       <c r="D14" s="34" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E14" s="32" t="s">
         <v>38</v>
@@ -6001,15 +6002,15 @@
       <c r="Q14"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B15" s="70"/>
-      <c r="C15" s="70"/>
+      <c r="B15" s="71"/>
+      <c r="C15" s="71"/>
       <c r="F15" s="13"/>
       <c r="O15"/>
       <c r="Q15"/>
     </row>
     <row r="16" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="70"/>
-      <c r="C16" s="70"/>
+      <c r="B16" s="71"/>
+      <c r="C16" s="71"/>
       <c r="F16" s="13"/>
       <c r="H16" s="73" t="s">
         <v>19</v>
@@ -6020,7 +6021,7 @@
       <c r="L16" s="73"/>
       <c r="M16" s="73"/>
       <c r="O16" s="73" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P16" s="73"/>
       <c r="Q16" s="73"/>
@@ -6029,8 +6030,8 @@
       <c r="T16" s="73"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B17" s="70"/>
-      <c r="C17" s="70"/>
+      <c r="B17" s="71"/>
+      <c r="C17" s="71"/>
       <c r="F17" s="13"/>
       <c r="H17" s="16" t="s">
         <v>4</v>
@@ -6070,8 +6071,8 @@
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B18" s="70"/>
-      <c r="C18" s="70"/>
+      <c r="B18" s="71"/>
+      <c r="C18" s="71"/>
       <c r="F18" s="13"/>
       <c r="H18" s="14">
         <f>COUNTIF(H12:H14,"O")</f>
@@ -6123,26 +6124,26 @@
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B19" s="70"/>
-      <c r="C19" s="70"/>
+      <c r="B19" s="71"/>
+      <c r="C19" s="71"/>
       <c r="F19" s="13"/>
       <c r="O19"/>
       <c r="Q19"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B20" s="70"/>
-      <c r="C20" s="70"/>
+      <c r="B20" s="71"/>
+      <c r="C20" s="71"/>
       <c r="F20" s="13"/>
-      <c r="H20" s="71" t="s">
+      <c r="H20" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="I20" s="71"/>
-      <c r="J20" s="71"/>
-      <c r="K20" s="71"/>
-      <c r="L20" s="71"/>
-      <c r="M20" s="71"/>
+      <c r="I20" s="72"/>
+      <c r="J20" s="72"/>
+      <c r="K20" s="72"/>
+      <c r="L20" s="72"/>
+      <c r="M20" s="72"/>
       <c r="O20" s="73" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P20" s="73"/>
       <c r="Q20" s="73"/>
@@ -6151,8 +6152,8 @@
       <c r="T20" s="73"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B21" s="70"/>
-      <c r="C21" s="70"/>
+      <c r="B21" s="71"/>
+      <c r="C21" s="71"/>
       <c r="F21" s="13"/>
       <c r="H21" s="16" t="s">
         <v>4</v>
@@ -6192,8 +6193,8 @@
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B22" s="70"/>
-      <c r="C22" s="70"/>
+      <c r="B22" s="71"/>
+      <c r="C22" s="71"/>
       <c r="F22" s="13"/>
       <c r="H22" s="14">
         <f>H18+O18+O22</f>
@@ -6245,15 +6246,15 @@
       </c>
     </row>
     <row r="23" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="70"/>
-      <c r="C23" s="70"/>
+      <c r="B23" s="71"/>
+      <c r="C23" s="71"/>
       <c r="F23" s="13"/>
       <c r="O23"/>
       <c r="Q23"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B24" s="70"/>
-      <c r="C24" s="70"/>
+      <c r="B24" s="71"/>
+      <c r="C24" s="71"/>
       <c r="F24" s="13"/>
       <c r="H24" s="43"/>
       <c r="J24" s="43"/>
@@ -6290,10 +6291,10 @@
       <c r="A26" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="79" t="s">
+      <c r="B26" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="79"/>
+      <c r="C26" s="78"/>
       <c r="D26" s="17" t="s">
         <v>1</v>
       </c>
@@ -6331,18 +6332,18 @@
       <c r="A27" s="30">
         <v>4</v>
       </c>
-      <c r="B27" s="80" t="s">
+      <c r="B27" s="79" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="80"/>
+      <c r="C27" s="79"/>
       <c r="D27" s="34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E27" s="32" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F27" s="29" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G27" s="30" t="s">
         <v>32</v>
@@ -6351,13 +6352,13 @@
         <v>10</v>
       </c>
       <c r="I27" s="44" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J27" s="31" t="s">
         <v>12</v>
       </c>
       <c r="K27" s="54" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L27" s="31" t="s">
         <v>12</v>
@@ -6375,13 +6376,13 @@
       </c>
       <c r="C28" s="81"/>
       <c r="D28" s="34" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E28" s="32" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F28" s="29" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G28" s="30" t="s">
         <v>32</v>
@@ -6390,13 +6391,13 @@
         <v>10</v>
       </c>
       <c r="I28" s="44" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J28" s="31" t="s">
         <v>10</v>
       </c>
       <c r="K28" s="54" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L28" s="31" t="s">
         <v>12</v>
@@ -6409,18 +6410,18 @@
       <c r="A29" s="58">
         <v>6</v>
       </c>
-      <c r="B29" s="80" t="s">
+      <c r="B29" s="79" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="80"/>
+      <c r="C29" s="79"/>
       <c r="D29" s="34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E29" s="32" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F29" s="29" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G29" s="58" t="s">
         <v>32</v>
@@ -6449,13 +6450,13 @@
       </c>
       <c r="C30" s="81"/>
       <c r="D30" s="34" t="s">
+        <v>140</v>
+      </c>
+      <c r="E30" s="32" t="s">
+        <v>138</v>
+      </c>
+      <c r="F30" s="29" t="s">
         <v>141</v>
-      </c>
-      <c r="E30" s="32" t="s">
-        <v>139</v>
-      </c>
-      <c r="F30" s="29" t="s">
-        <v>142</v>
       </c>
       <c r="G30" s="58" t="s">
         <v>32</v>
@@ -6477,8 +6478,8 @@
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="27"/>
-      <c r="B31" s="82"/>
-      <c r="C31" s="82"/>
+      <c r="B31" s="85"/>
+      <c r="C31" s="85"/>
       <c r="D31" s="28"/>
       <c r="E31" s="29"/>
       <c r="F31" s="29"/>
@@ -6493,8 +6494,8 @@
       <c r="Q31" s="23"/>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B32" s="70"/>
-      <c r="C32" s="70"/>
+      <c r="B32" s="71"/>
+      <c r="C32" s="71"/>
       <c r="F32" s="13"/>
       <c r="H32" s="23"/>
       <c r="J32" s="23"/>
@@ -6503,8 +6504,8 @@
       <c r="Q32" s="23"/>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B33" s="70"/>
-      <c r="C33" s="70"/>
+      <c r="B33" s="71"/>
+      <c r="C33" s="71"/>
       <c r="F33" s="13"/>
       <c r="H33" s="73" t="s">
         <v>19</v>
@@ -6515,7 +6516,7 @@
       <c r="L33" s="73"/>
       <c r="M33" s="73"/>
       <c r="O33" s="73" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P33" s="73"/>
       <c r="Q33" s="73"/>
@@ -6524,8 +6525,8 @@
       <c r="T33" s="73"/>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B34" s="70"/>
-      <c r="C34" s="70"/>
+      <c r="B34" s="71"/>
+      <c r="C34" s="71"/>
       <c r="F34" s="13"/>
       <c r="H34" s="16" t="s">
         <v>4</v>
@@ -6565,8 +6566,8 @@
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B35" s="70"/>
-      <c r="C35" s="70"/>
+      <c r="B35" s="71"/>
+      <c r="C35" s="71"/>
       <c r="F35" s="13"/>
       <c r="H35" s="14">
         <f>COUNTIF(H27:H31,"O")</f>
@@ -6618,8 +6619,8 @@
       </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B36" s="70"/>
-      <c r="C36" s="70"/>
+      <c r="B36" s="71"/>
+      <c r="C36" s="71"/>
       <c r="F36" s="13"/>
       <c r="H36" s="43"/>
       <c r="J36" s="43"/>
@@ -6628,19 +6629,19 @@
       <c r="Q36"/>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B37" s="70"/>
-      <c r="C37" s="70"/>
+      <c r="B37" s="71"/>
+      <c r="C37" s="71"/>
       <c r="F37" s="13"/>
-      <c r="H37" s="71" t="s">
+      <c r="H37" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="I37" s="71"/>
-      <c r="J37" s="71"/>
-      <c r="K37" s="71"/>
-      <c r="L37" s="71"/>
-      <c r="M37" s="71"/>
+      <c r="I37" s="72"/>
+      <c r="J37" s="72"/>
+      <c r="K37" s="72"/>
+      <c r="L37" s="72"/>
+      <c r="M37" s="72"/>
       <c r="O37" s="73" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P37" s="73"/>
       <c r="Q37" s="73"/>
@@ -6649,8 +6650,8 @@
       <c r="T37" s="73"/>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B38" s="70"/>
-      <c r="C38" s="70"/>
+      <c r="B38" s="71"/>
+      <c r="C38" s="71"/>
       <c r="F38" s="13"/>
       <c r="H38" s="16" t="s">
         <v>4</v>
@@ -6690,8 +6691,8 @@
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B39" s="70"/>
-      <c r="C39" s="70"/>
+      <c r="B39" s="71"/>
+      <c r="C39" s="71"/>
       <c r="F39" s="13"/>
       <c r="H39" s="14">
         <f>H35+O35+O39</f>
@@ -6743,8 +6744,8 @@
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B40" s="70"/>
-      <c r="C40" s="70"/>
+      <c r="B40" s="71"/>
+      <c r="C40" s="71"/>
       <c r="F40" s="13"/>
       <c r="H40" s="23"/>
       <c r="J40" s="23"/>
@@ -6779,10 +6780,10 @@
       <c r="A42" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B42" s="79" t="s">
+      <c r="B42" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="C42" s="79"/>
+      <c r="C42" s="78"/>
       <c r="D42" s="26" t="s">
         <v>1</v>
       </c>
@@ -6818,12 +6819,12 @@
       <c r="A43" s="35">
         <v>8</v>
       </c>
-      <c r="B43" s="80" t="s">
+      <c r="B43" s="79" t="s">
         <v>30</v>
       </c>
-      <c r="C43" s="80"/>
+      <c r="C43" s="79"/>
       <c r="D43" s="34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E43" s="32" t="s">
         <v>42</v>
@@ -6838,7 +6839,7 @@
         <v>12</v>
       </c>
       <c r="I43" s="44" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J43" s="31" t="s">
         <v>12</v>
@@ -6858,13 +6859,13 @@
       </c>
       <c r="C44" s="81"/>
       <c r="D44" s="34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E44" s="32" t="s">
         <v>43</v>
       </c>
       <c r="F44" s="29" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G44" s="35" t="s">
         <v>32</v>
@@ -6886,15 +6887,15 @@
       <c r="A45" s="35">
         <v>10</v>
       </c>
-      <c r="B45" s="78" t="s">
+      <c r="B45" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="C45" s="78"/>
+      <c r="C45" s="70"/>
       <c r="D45" s="34" t="s">
+        <v>158</v>
+      </c>
+      <c r="E45" s="32" t="s">
         <v>45</v>
-      </c>
-      <c r="E45" s="32" t="s">
-        <v>46</v>
       </c>
       <c r="F45" s="29" t="s">
         <v>44</v>
@@ -6919,18 +6920,18 @@
       <c r="A46" s="68">
         <v>11</v>
       </c>
-      <c r="B46" s="78" t="s">
+      <c r="B46" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="C46" s="78"/>
+      <c r="C46" s="70"/>
       <c r="D46" s="34" t="s">
+        <v>149</v>
+      </c>
+      <c r="E46" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="F46" s="29" t="s">
         <v>150</v>
-      </c>
-      <c r="E46" s="32" t="s">
-        <v>149</v>
-      </c>
-      <c r="F46" s="29" t="s">
-        <v>151</v>
       </c>
       <c r="G46" s="68" t="s">
         <v>32</v>
@@ -6951,16 +6952,16 @@
       <c r="Q46" s="67"/>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B47" s="70"/>
-      <c r="C47" s="70"/>
+      <c r="B47" s="71"/>
+      <c r="C47" s="71"/>
       <c r="F47" s="13"/>
       <c r="H47" s="24"/>
       <c r="J47" s="24"/>
       <c r="L47" s="24"/>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B48" s="70"/>
-      <c r="C48" s="70"/>
+      <c r="B48" s="71"/>
+      <c r="C48" s="71"/>
       <c r="F48" s="13"/>
       <c r="H48" s="73" t="s">
         <v>19</v>
@@ -6971,7 +6972,7 @@
       <c r="L48" s="73"/>
       <c r="M48" s="73"/>
       <c r="O48" s="73" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P48" s="73"/>
       <c r="Q48" s="73"/>
@@ -6980,8 +6981,8 @@
       <c r="T48" s="73"/>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B49" s="70"/>
-      <c r="C49" s="70"/>
+      <c r="B49" s="71"/>
+      <c r="C49" s="71"/>
       <c r="F49" s="13"/>
       <c r="H49" s="16" t="s">
         <v>4</v>
@@ -7021,8 +7022,8 @@
       </c>
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B50" s="70"/>
-      <c r="C50" s="70"/>
+      <c r="B50" s="71"/>
+      <c r="C50" s="71"/>
       <c r="F50" s="13"/>
       <c r="H50" s="14">
         <f>COUNTIF(H43:H45,"O")</f>
@@ -7074,8 +7075,8 @@
       </c>
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B51" s="70"/>
-      <c r="C51" s="70"/>
+      <c r="B51" s="71"/>
+      <c r="C51" s="71"/>
       <c r="F51" s="13"/>
       <c r="H51" s="43"/>
       <c r="J51" s="43"/>
@@ -7084,19 +7085,19 @@
       <c r="Q51"/>
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B52" s="70"/>
-      <c r="C52" s="70"/>
+      <c r="B52" s="71"/>
+      <c r="C52" s="71"/>
       <c r="F52" s="13"/>
-      <c r="H52" s="71" t="s">
+      <c r="H52" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="I52" s="71"/>
-      <c r="J52" s="71"/>
-      <c r="K52" s="71"/>
-      <c r="L52" s="71"/>
-      <c r="M52" s="71"/>
+      <c r="I52" s="72"/>
+      <c r="J52" s="72"/>
+      <c r="K52" s="72"/>
+      <c r="L52" s="72"/>
+      <c r="M52" s="72"/>
       <c r="O52" s="73" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P52" s="73"/>
       <c r="Q52" s="73"/>
@@ -7105,8 +7106,8 @@
       <c r="T52" s="73"/>
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B53" s="70"/>
-      <c r="C53" s="70"/>
+      <c r="B53" s="71"/>
+      <c r="C53" s="71"/>
       <c r="F53" s="13"/>
       <c r="H53" s="16" t="s">
         <v>4</v>
@@ -7146,8 +7147,8 @@
       </c>
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B54" s="70"/>
-      <c r="C54" s="70"/>
+      <c r="B54" s="71"/>
+      <c r="C54" s="71"/>
       <c r="F54" s="13"/>
       <c r="H54" s="14">
         <f>H50+O50+O54</f>
@@ -7199,8 +7200,8 @@
       </c>
     </row>
     <row r="55" spans="1:20" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="72"/>
-      <c r="C55" s="72"/>
+      <c r="B55" s="80"/>
+      <c r="C55" s="80"/>
       <c r="F55" s="41"/>
       <c r="H55" s="42"/>
       <c r="J55" s="42"/>
@@ -7210,7 +7211,7 @@
     </row>
     <row r="56" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A56" s="74" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B56" s="74"/>
       <c r="C56" s="74"/>
@@ -7235,10 +7236,10 @@
       <c r="A57" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B57" s="79" t="s">
+      <c r="B57" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="C57" s="79"/>
+      <c r="C57" s="78"/>
       <c r="D57" s="26" t="s">
         <v>1</v>
       </c>
@@ -7274,18 +7275,18 @@
       <c r="A58" s="35">
         <v>12</v>
       </c>
-      <c r="B58" s="80" t="s">
+      <c r="B58" s="79" t="s">
+        <v>47</v>
+      </c>
+      <c r="C58" s="79"/>
+      <c r="D58" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="C58" s="80"/>
-      <c r="D58" s="34" t="s">
+      <c r="E58" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="E58" s="32" t="s">
+      <c r="F58" s="29" t="s">
         <v>50</v>
-      </c>
-      <c r="F58" s="29" t="s">
-        <v>51</v>
       </c>
       <c r="G58" s="35" t="s">
         <v>32</v>
@@ -7308,17 +7309,17 @@
         <v>13</v>
       </c>
       <c r="B59" s="81" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C59" s="81"/>
       <c r="D59" s="34" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E59" s="32" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F59" s="29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G59" s="35" t="s">
         <v>32</v>
@@ -7335,20 +7336,20 @@
         <v>12</v>
       </c>
       <c r="M59" s="69" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B60" s="70"/>
-      <c r="C60" s="70"/>
+      <c r="B60" s="71"/>
+      <c r="C60" s="71"/>
       <c r="F60" s="13"/>
       <c r="H60" s="24"/>
       <c r="J60" s="24"/>
       <c r="L60" s="24"/>
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B61" s="70"/>
-      <c r="C61" s="70"/>
+      <c r="B61" s="71"/>
+      <c r="C61" s="71"/>
       <c r="F61" s="13"/>
       <c r="H61" s="73" t="s">
         <v>19</v>
@@ -7359,7 +7360,7 @@
       <c r="L61" s="73"/>
       <c r="M61" s="73"/>
       <c r="O61" s="73" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P61" s="73"/>
       <c r="Q61" s="73"/>
@@ -7368,8 +7369,8 @@
       <c r="T61" s="73"/>
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B62" s="70"/>
-      <c r="C62" s="70"/>
+      <c r="B62" s="71"/>
+      <c r="C62" s="71"/>
       <c r="F62" s="13"/>
       <c r="H62" s="16" t="s">
         <v>4</v>
@@ -7409,8 +7410,8 @@
       </c>
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B63" s="70"/>
-      <c r="C63" s="70"/>
+      <c r="B63" s="71"/>
+      <c r="C63" s="71"/>
       <c r="F63" s="13"/>
       <c r="H63" s="14">
         <f>COUNTIF(H58:H59,"O")</f>
@@ -7462,8 +7463,8 @@
       </c>
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B64" s="70"/>
-      <c r="C64" s="70"/>
+      <c r="B64" s="71"/>
+      <c r="C64" s="71"/>
       <c r="F64" s="13"/>
       <c r="H64" s="43"/>
       <c r="J64" s="43"/>
@@ -7472,19 +7473,19 @@
       <c r="Q64"/>
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B65" s="70"/>
-      <c r="C65" s="70"/>
+      <c r="B65" s="71"/>
+      <c r="C65" s="71"/>
       <c r="F65" s="13"/>
-      <c r="H65" s="71" t="s">
+      <c r="H65" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="I65" s="71"/>
-      <c r="J65" s="71"/>
-      <c r="K65" s="71"/>
-      <c r="L65" s="71"/>
-      <c r="M65" s="71"/>
+      <c r="I65" s="72"/>
+      <c r="J65" s="72"/>
+      <c r="K65" s="72"/>
+      <c r="L65" s="72"/>
+      <c r="M65" s="72"/>
       <c r="O65" s="73" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P65" s="73"/>
       <c r="Q65" s="73"/>
@@ -7493,8 +7494,8 @@
       <c r="T65" s="73"/>
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B66" s="70"/>
-      <c r="C66" s="70"/>
+      <c r="B66" s="71"/>
+      <c r="C66" s="71"/>
       <c r="F66" s="13"/>
       <c r="H66" s="16" t="s">
         <v>4</v>
@@ -7534,8 +7535,8 @@
       </c>
     </row>
     <row r="67" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B67" s="70"/>
-      <c r="C67" s="70"/>
+      <c r="B67" s="71"/>
+      <c r="C67" s="71"/>
       <c r="F67" s="13"/>
       <c r="H67" s="14">
         <f>H63+O63+O67</f>
@@ -7588,8 +7589,8 @@
     </row>
     <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" s="40"/>
-      <c r="B68" s="72"/>
-      <c r="C68" s="72"/>
+      <c r="B68" s="80"/>
+      <c r="C68" s="80"/>
       <c r="D68" s="40"/>
       <c r="E68" s="40"/>
       <c r="F68" s="41"/>
@@ -7604,7 +7605,7 @@
     </row>
     <row r="69" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A69" s="74" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B69" s="74"/>
       <c r="C69" s="74"/>
@@ -7631,10 +7632,10 @@
       <c r="A70" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B70" s="79" t="s">
+      <c r="B70" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="C70" s="79"/>
+      <c r="C70" s="78"/>
       <c r="D70" s="38" t="s">
         <v>1</v>
       </c>
@@ -7672,18 +7673,18 @@
       <c r="A71" s="39">
         <v>14</v>
       </c>
-      <c r="B71" s="80" t="s">
+      <c r="B71" s="79" t="s">
+        <v>52</v>
+      </c>
+      <c r="C71" s="79"/>
+      <c r="D71" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="C71" s="80"/>
-      <c r="D71" s="34" t="s">
+      <c r="E71" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="E71" s="32" t="s">
+      <c r="F71" s="29" t="s">
         <v>55</v>
-      </c>
-      <c r="F71" s="29" t="s">
-        <v>56</v>
       </c>
       <c r="G71" s="39" t="s">
         <v>32</v>
@@ -7704,8 +7705,8 @@
       <c r="Q71" s="37"/>
     </row>
     <row r="72" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B72" s="70"/>
-      <c r="C72" s="70"/>
+      <c r="B72" s="71"/>
+      <c r="C72" s="71"/>
       <c r="F72" s="13"/>
       <c r="H72" s="37"/>
       <c r="J72" s="37"/>
@@ -7714,8 +7715,8 @@
       <c r="Q72" s="37"/>
     </row>
     <row r="73" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B73" s="70"/>
-      <c r="C73" s="70"/>
+      <c r="B73" s="71"/>
+      <c r="C73" s="71"/>
       <c r="F73" s="13"/>
       <c r="H73" s="73" t="s">
         <v>19</v>
@@ -7726,7 +7727,7 @@
       <c r="L73" s="73"/>
       <c r="M73" s="73"/>
       <c r="O73" s="73" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P73" s="73"/>
       <c r="Q73" s="73"/>
@@ -7735,8 +7736,8 @@
       <c r="T73" s="73"/>
     </row>
     <row r="74" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B74" s="70"/>
-      <c r="C74" s="70"/>
+      <c r="B74" s="71"/>
+      <c r="C74" s="71"/>
       <c r="F74" s="13"/>
       <c r="H74" s="16" t="s">
         <v>4</v>
@@ -7776,8 +7777,8 @@
       </c>
     </row>
     <row r="75" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B75" s="70"/>
-      <c r="C75" s="70"/>
+      <c r="B75" s="71"/>
+      <c r="C75" s="71"/>
       <c r="F75" s="13"/>
       <c r="H75" s="14">
         <f>COUNTIF(H69:H71,"O")</f>
@@ -7829,8 +7830,8 @@
       </c>
     </row>
     <row r="76" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B76" s="70"/>
-      <c r="C76" s="70"/>
+      <c r="B76" s="71"/>
+      <c r="C76" s="71"/>
       <c r="F76" s="13"/>
       <c r="H76" s="43"/>
       <c r="J76" s="43"/>
@@ -7839,19 +7840,19 @@
       <c r="Q76"/>
     </row>
     <row r="77" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B77" s="70"/>
-      <c r="C77" s="70"/>
+      <c r="B77" s="71"/>
+      <c r="C77" s="71"/>
       <c r="F77" s="13"/>
-      <c r="H77" s="71" t="s">
+      <c r="H77" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="I77" s="71"/>
-      <c r="J77" s="71"/>
-      <c r="K77" s="71"/>
-      <c r="L77" s="71"/>
-      <c r="M77" s="71"/>
+      <c r="I77" s="72"/>
+      <c r="J77" s="72"/>
+      <c r="K77" s="72"/>
+      <c r="L77" s="72"/>
+      <c r="M77" s="72"/>
       <c r="O77" s="73" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P77" s="73"/>
       <c r="Q77" s="73"/>
@@ -7860,8 +7861,8 @@
       <c r="T77" s="73"/>
     </row>
     <row r="78" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B78" s="70"/>
-      <c r="C78" s="70"/>
+      <c r="B78" s="71"/>
+      <c r="C78" s="71"/>
       <c r="F78" s="13"/>
       <c r="H78" s="16" t="s">
         <v>4</v>
@@ -7901,8 +7902,8 @@
       </c>
     </row>
     <row r="79" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B79" s="70"/>
-      <c r="C79" s="70"/>
+      <c r="B79" s="71"/>
+      <c r="C79" s="71"/>
       <c r="F79" s="13"/>
       <c r="H79" s="14">
         <f>H75+O75+O79</f>
@@ -7955,8 +7956,8 @@
     </row>
     <row r="80" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A80" s="40"/>
-      <c r="B80" s="72"/>
-      <c r="C80" s="72"/>
+      <c r="B80" s="80"/>
+      <c r="C80" s="80"/>
       <c r="D80" s="40"/>
       <c r="E80" s="40"/>
       <c r="F80" s="41"/>
@@ -7973,7 +7974,7 @@
     </row>
     <row r="81" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A81" s="74" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B81" s="74"/>
       <c r="C81" s="74"/>
@@ -8000,10 +8001,10 @@
       <c r="A82" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B82" s="79" t="s">
+      <c r="B82" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="C82" s="79"/>
+      <c r="C82" s="78"/>
       <c r="D82" s="38" t="s">
         <v>1</v>
       </c>
@@ -8041,18 +8042,18 @@
       <c r="A83" s="39">
         <v>15</v>
       </c>
-      <c r="B83" s="80" t="s">
+      <c r="B83" s="79" t="s">
+        <v>57</v>
+      </c>
+      <c r="C83" s="79"/>
+      <c r="D83" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="C83" s="80"/>
-      <c r="D83" s="34" t="s">
+      <c r="E83" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="E83" s="32" t="s">
+      <c r="F83" s="29" t="s">
         <v>60</v>
-      </c>
-      <c r="F83" s="29" t="s">
-        <v>61</v>
       </c>
       <c r="G83" s="39" t="s">
         <v>32</v>
@@ -8073,8 +8074,8 @@
       <c r="Q83" s="37"/>
     </row>
     <row r="84" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B84" s="70"/>
-      <c r="C84" s="70"/>
+      <c r="B84" s="71"/>
+      <c r="C84" s="71"/>
       <c r="F84" s="13"/>
       <c r="H84" s="37"/>
       <c r="J84" s="37"/>
@@ -8083,8 +8084,8 @@
       <c r="Q84" s="37"/>
     </row>
     <row r="85" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B85" s="70"/>
-      <c r="C85" s="70"/>
+      <c r="B85" s="71"/>
+      <c r="C85" s="71"/>
       <c r="F85" s="13"/>
       <c r="H85" s="73" t="s">
         <v>19</v>
@@ -8095,7 +8096,7 @@
       <c r="L85" s="73"/>
       <c r="M85" s="73"/>
       <c r="O85" s="73" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P85" s="73"/>
       <c r="Q85" s="73"/>
@@ -8104,8 +8105,8 @@
       <c r="T85" s="73"/>
     </row>
     <row r="86" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B86" s="70"/>
-      <c r="C86" s="70"/>
+      <c r="B86" s="71"/>
+      <c r="C86" s="71"/>
       <c r="F86" s="13"/>
       <c r="H86" s="16" t="s">
         <v>4</v>
@@ -8145,8 +8146,8 @@
       </c>
     </row>
     <row r="87" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B87" s="70"/>
-      <c r="C87" s="70"/>
+      <c r="B87" s="71"/>
+      <c r="C87" s="71"/>
       <c r="F87" s="13"/>
       <c r="H87" s="14">
         <f>COUNTIF(H81:H83,"O")</f>
@@ -8198,8 +8199,8 @@
       </c>
     </row>
     <row r="88" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B88" s="70"/>
-      <c r="C88" s="70"/>
+      <c r="B88" s="71"/>
+      <c r="C88" s="71"/>
       <c r="F88" s="13"/>
       <c r="H88" s="43"/>
       <c r="J88" s="43"/>
@@ -8208,19 +8209,19 @@
       <c r="Q88"/>
     </row>
     <row r="89" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B89" s="70"/>
-      <c r="C89" s="70"/>
+      <c r="B89" s="71"/>
+      <c r="C89" s="71"/>
       <c r="F89" s="13"/>
-      <c r="H89" s="71" t="s">
+      <c r="H89" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="I89" s="71"/>
-      <c r="J89" s="71"/>
-      <c r="K89" s="71"/>
-      <c r="L89" s="71"/>
-      <c r="M89" s="71"/>
+      <c r="I89" s="72"/>
+      <c r="J89" s="72"/>
+      <c r="K89" s="72"/>
+      <c r="L89" s="72"/>
+      <c r="M89" s="72"/>
       <c r="O89" s="73" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P89" s="73"/>
       <c r="Q89" s="73"/>
@@ -8229,8 +8230,8 @@
       <c r="T89" s="73"/>
     </row>
     <row r="90" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B90" s="70"/>
-      <c r="C90" s="70"/>
+      <c r="B90" s="71"/>
+      <c r="C90" s="71"/>
       <c r="F90" s="13"/>
       <c r="H90" s="16" t="s">
         <v>4</v>
@@ -8270,8 +8271,8 @@
       </c>
     </row>
     <row r="91" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B91" s="70"/>
-      <c r="C91" s="70"/>
+      <c r="B91" s="71"/>
+      <c r="C91" s="71"/>
       <c r="F91" s="13"/>
       <c r="H91" s="14">
         <f>H87+O87+O91</f>
@@ -8324,8 +8325,8 @@
     </row>
     <row r="92" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A92" s="40"/>
-      <c r="B92" s="72"/>
-      <c r="C92" s="72"/>
+      <c r="B92" s="80"/>
+      <c r="C92" s="80"/>
       <c r="D92" s="40"/>
       <c r="E92" s="40"/>
       <c r="F92" s="41"/>
@@ -8342,7 +8343,7 @@
     </row>
     <row r="93" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A93" s="74" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B93" s="74"/>
       <c r="C93" s="74"/>
@@ -8369,10 +8370,10 @@
       <c r="A94" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B94" s="79" t="s">
+      <c r="B94" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="C94" s="79"/>
+      <c r="C94" s="78"/>
       <c r="D94" s="38" t="s">
         <v>1</v>
       </c>
@@ -8410,18 +8411,18 @@
       <c r="A95" s="39">
         <v>16</v>
       </c>
-      <c r="B95" s="80" t="s">
-        <v>62</v>
-      </c>
-      <c r="C95" s="80"/>
+      <c r="B95" s="79" t="s">
+        <v>61</v>
+      </c>
+      <c r="C95" s="79"/>
       <c r="D95" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="E95" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="E95" s="32" t="s">
+      <c r="F95" s="29" t="s">
         <v>93</v>
-      </c>
-      <c r="F95" s="29" t="s">
-        <v>94</v>
       </c>
       <c r="G95" s="39" t="s">
         <v>32</v>
@@ -8446,17 +8447,17 @@
         <v>17</v>
       </c>
       <c r="B96" s="81" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C96" s="81"/>
       <c r="D96" s="34" t="s">
+        <v>124</v>
+      </c>
+      <c r="E96" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="F96" s="29" t="s">
         <v>125</v>
-      </c>
-      <c r="E96" s="32" t="s">
-        <v>95</v>
-      </c>
-      <c r="F96" s="29" t="s">
-        <v>126</v>
       </c>
       <c r="G96" s="39" t="s">
         <v>32</v>
@@ -8477,8 +8478,8 @@
       <c r="Q96" s="37"/>
     </row>
     <row r="97" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B97" s="70"/>
-      <c r="C97" s="70"/>
+      <c r="B97" s="71"/>
+      <c r="C97" s="71"/>
       <c r="F97" s="13"/>
       <c r="H97" s="37"/>
       <c r="J97" s="37"/>
@@ -8487,8 +8488,8 @@
       <c r="Q97" s="37"/>
     </row>
     <row r="98" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B98" s="70"/>
-      <c r="C98" s="70"/>
+      <c r="B98" s="71"/>
+      <c r="C98" s="71"/>
       <c r="F98" s="13"/>
       <c r="H98" s="73" t="s">
         <v>19</v>
@@ -8499,7 +8500,7 @@
       <c r="L98" s="73"/>
       <c r="M98" s="73"/>
       <c r="O98" s="73" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P98" s="73"/>
       <c r="Q98" s="73"/>
@@ -8508,8 +8509,8 @@
       <c r="T98" s="73"/>
     </row>
     <row r="99" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B99" s="70"/>
-      <c r="C99" s="70"/>
+      <c r="B99" s="71"/>
+      <c r="C99" s="71"/>
       <c r="F99" s="13"/>
       <c r="H99" s="16" t="s">
         <v>4</v>
@@ -8549,8 +8550,8 @@
       </c>
     </row>
     <row r="100" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B100" s="70"/>
-      <c r="C100" s="70"/>
+      <c r="B100" s="71"/>
+      <c r="C100" s="71"/>
       <c r="F100" s="13"/>
       <c r="H100" s="14">
         <f>COUNTIF(H95:H96,"O")</f>
@@ -8602,8 +8603,8 @@
       </c>
     </row>
     <row r="101" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B101" s="70"/>
-      <c r="C101" s="70"/>
+      <c r="B101" s="71"/>
+      <c r="C101" s="71"/>
       <c r="F101" s="13"/>
       <c r="H101" s="43"/>
       <c r="J101" s="43"/>
@@ -8612,19 +8613,19 @@
       <c r="Q101"/>
     </row>
     <row r="102" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B102" s="70"/>
-      <c r="C102" s="70"/>
+      <c r="B102" s="71"/>
+      <c r="C102" s="71"/>
       <c r="F102" s="13"/>
-      <c r="H102" s="71" t="s">
+      <c r="H102" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="I102" s="71"/>
-      <c r="J102" s="71"/>
-      <c r="K102" s="71"/>
-      <c r="L102" s="71"/>
-      <c r="M102" s="71"/>
+      <c r="I102" s="72"/>
+      <c r="J102" s="72"/>
+      <c r="K102" s="72"/>
+      <c r="L102" s="72"/>
+      <c r="M102" s="72"/>
       <c r="O102" s="73" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P102" s="73"/>
       <c r="Q102" s="73"/>
@@ -8633,8 +8634,8 @@
       <c r="T102" s="73"/>
     </row>
     <row r="103" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B103" s="70"/>
-      <c r="C103" s="70"/>
+      <c r="B103" s="71"/>
+      <c r="C103" s="71"/>
       <c r="F103" s="13"/>
       <c r="H103" s="16" t="s">
         <v>4</v>
@@ -8674,8 +8675,8 @@
       </c>
     </row>
     <row r="104" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B104" s="70"/>
-      <c r="C104" s="70"/>
+      <c r="B104" s="71"/>
+      <c r="C104" s="71"/>
       <c r="F104" s="13"/>
       <c r="H104" s="14">
         <f>H100+O100+O104</f>
@@ -8728,8 +8729,8 @@
     </row>
     <row r="105" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A105" s="40"/>
-      <c r="B105" s="72"/>
-      <c r="C105" s="72"/>
+      <c r="B105" s="80"/>
+      <c r="C105" s="80"/>
       <c r="D105" s="40"/>
       <c r="E105" s="40"/>
       <c r="F105" s="41"/>
@@ -8746,7 +8747,7 @@
     </row>
     <row r="106" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A106" s="74" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B106" s="74"/>
       <c r="C106" s="74"/>
@@ -8773,10 +8774,10 @@
       <c r="A107" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B107" s="79" t="s">
+      <c r="B107" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="C107" s="79"/>
+      <c r="C107" s="78"/>
       <c r="D107" s="49" t="s">
         <v>1</v>
       </c>
@@ -8814,18 +8815,18 @@
       <c r="A108" s="48">
         <v>18</v>
       </c>
-      <c r="B108" s="80" t="s">
-        <v>105</v>
-      </c>
-      <c r="C108" s="80"/>
+      <c r="B108" s="79" t="s">
+        <v>104</v>
+      </c>
+      <c r="C108" s="79"/>
       <c r="D108" s="50" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E108" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="F108" s="29" t="s">
         <v>96</v>
-      </c>
-      <c r="F108" s="29" t="s">
-        <v>97</v>
       </c>
       <c r="G108" s="48" t="s">
         <v>32</v>
@@ -8850,17 +8851,17 @@
         <v>19</v>
       </c>
       <c r="B109" s="81" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C109" s="81"/>
       <c r="D109" s="34" t="s">
+        <v>127</v>
+      </c>
+      <c r="E109" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="F109" s="29" t="s">
         <v>128</v>
-      </c>
-      <c r="E109" s="32" t="s">
-        <v>95</v>
-      </c>
-      <c r="F109" s="29" t="s">
-        <v>129</v>
       </c>
       <c r="G109" s="48" t="s">
         <v>32</v>
@@ -8881,8 +8882,8 @@
       <c r="Q109" s="46"/>
     </row>
     <row r="110" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B110" s="70"/>
-      <c r="C110" s="70"/>
+      <c r="B110" s="71"/>
+      <c r="C110" s="71"/>
       <c r="F110" s="13"/>
       <c r="H110" s="46"/>
       <c r="J110" s="46"/>
@@ -8891,8 +8892,8 @@
       <c r="Q110" s="46"/>
     </row>
     <row r="111" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B111" s="70"/>
-      <c r="C111" s="70"/>
+      <c r="B111" s="71"/>
+      <c r="C111" s="71"/>
       <c r="F111" s="13"/>
       <c r="H111" s="73" t="s">
         <v>19</v>
@@ -8903,7 +8904,7 @@
       <c r="L111" s="73"/>
       <c r="M111" s="73"/>
       <c r="O111" s="73" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P111" s="73"/>
       <c r="Q111" s="73"/>
@@ -8912,8 +8913,8 @@
       <c r="T111" s="73"/>
     </row>
     <row r="112" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B112" s="70"/>
-      <c r="C112" s="70"/>
+      <c r="B112" s="71"/>
+      <c r="C112" s="71"/>
       <c r="F112" s="13"/>
       <c r="H112" s="16" t="s">
         <v>4</v>
@@ -8953,8 +8954,8 @@
       </c>
     </row>
     <row r="113" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B113" s="70"/>
-      <c r="C113" s="70"/>
+      <c r="B113" s="71"/>
+      <c r="C113" s="71"/>
       <c r="F113" s="13"/>
       <c r="H113" s="14">
         <f>COUNTIF(H108:H109,"O")</f>
@@ -9006,8 +9007,8 @@
       </c>
     </row>
     <row r="114" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B114" s="70"/>
-      <c r="C114" s="70"/>
+      <c r="B114" s="71"/>
+      <c r="C114" s="71"/>
       <c r="F114" s="13"/>
       <c r="H114" s="46"/>
       <c r="J114" s="46"/>
@@ -9016,19 +9017,19 @@
       <c r="Q114"/>
     </row>
     <row r="115" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B115" s="70"/>
-      <c r="C115" s="70"/>
+      <c r="B115" s="71"/>
+      <c r="C115" s="71"/>
       <c r="F115" s="13"/>
-      <c r="H115" s="71" t="s">
+      <c r="H115" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="I115" s="71"/>
-      <c r="J115" s="71"/>
-      <c r="K115" s="71"/>
-      <c r="L115" s="71"/>
-      <c r="M115" s="71"/>
+      <c r="I115" s="72"/>
+      <c r="J115" s="72"/>
+      <c r="K115" s="72"/>
+      <c r="L115" s="72"/>
+      <c r="M115" s="72"/>
       <c r="O115" s="73" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P115" s="73"/>
       <c r="Q115" s="73"/>
@@ -9037,8 +9038,8 @@
       <c r="T115" s="73"/>
     </row>
     <row r="116" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B116" s="70"/>
-      <c r="C116" s="70"/>
+      <c r="B116" s="71"/>
+      <c r="C116" s="71"/>
       <c r="F116" s="13"/>
       <c r="H116" s="16" t="s">
         <v>4</v>
@@ -9078,8 +9079,8 @@
       </c>
     </row>
     <row r="117" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B117" s="70"/>
-      <c r="C117" s="70"/>
+      <c r="B117" s="71"/>
+      <c r="C117" s="71"/>
       <c r="F117" s="13"/>
       <c r="H117" s="14">
         <f>H113+O113+O117</f>
@@ -9149,7 +9150,7 @@
     </row>
     <row r="119" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A119" s="74" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B119" s="74"/>
       <c r="C119" s="74"/>
@@ -9176,10 +9177,10 @@
       <c r="A120" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="B120" s="79" t="s">
+      <c r="B120" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="C120" s="79"/>
+      <c r="C120" s="78"/>
       <c r="D120" s="66" t="s">
         <v>1</v>
       </c>
@@ -9217,18 +9218,18 @@
       <c r="A121" s="65">
         <v>20</v>
       </c>
-      <c r="B121" s="80" t="s">
+      <c r="B121" s="79" t="s">
+        <v>144</v>
+      </c>
+      <c r="C121" s="79"/>
+      <c r="D121" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="E121" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="F121" s="29" t="s">
         <v>145</v>
-      </c>
-      <c r="C121" s="80"/>
-      <c r="D121" s="50" t="s">
-        <v>147</v>
-      </c>
-      <c r="E121" s="32" t="s">
-        <v>96</v>
-      </c>
-      <c r="F121" s="29" t="s">
-        <v>146</v>
       </c>
       <c r="G121" s="65" t="s">
         <v>32</v>
@@ -9245,14 +9246,14 @@
         <v>12</v>
       </c>
       <c r="M121" s="31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="O121" s="63"/>
       <c r="Q121" s="63"/>
     </row>
     <row r="122" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B122" s="70"/>
-      <c r="C122" s="70"/>
+      <c r="B122" s="71"/>
+      <c r="C122" s="71"/>
       <c r="F122" s="13"/>
       <c r="H122" s="63"/>
       <c r="J122" s="63"/>
@@ -9261,8 +9262,8 @@
       <c r="Q122" s="63"/>
     </row>
     <row r="123" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B123" s="70"/>
-      <c r="C123" s="70"/>
+      <c r="B123" s="71"/>
+      <c r="C123" s="71"/>
       <c r="F123" s="13"/>
       <c r="H123" s="73" t="s">
         <v>19</v>
@@ -9273,7 +9274,7 @@
       <c r="L123" s="73"/>
       <c r="M123" s="73"/>
       <c r="O123" s="73" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P123" s="73"/>
       <c r="Q123" s="73"/>
@@ -9282,10 +9283,10 @@
       <c r="T123" s="73"/>
     </row>
     <row r="124" spans="1:20" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B124" s="70"/>
-      <c r="C124" s="70"/>
+      <c r="B124" s="71"/>
+      <c r="C124" s="71"/>
       <c r="E124" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F124" s="13"/>
       <c r="H124" s="16" t="s">
@@ -9326,8 +9327,8 @@
       </c>
     </row>
     <row r="125" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B125" s="70"/>
-      <c r="C125" s="70"/>
+      <c r="B125" s="71"/>
+      <c r="C125" s="71"/>
       <c r="F125" s="13"/>
       <c r="H125" s="14">
         <f>COUNTIF(H121:H121,"O")</f>
@@ -9379,8 +9380,8 @@
       </c>
     </row>
     <row r="126" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B126" s="70"/>
-      <c r="C126" s="70"/>
+      <c r="B126" s="71"/>
+      <c r="C126" s="71"/>
       <c r="F126" s="13"/>
       <c r="H126" s="63"/>
       <c r="J126" s="63"/>
@@ -9389,19 +9390,19 @@
       <c r="Q126"/>
     </row>
     <row r="127" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B127" s="70"/>
-      <c r="C127" s="70"/>
+      <c r="B127" s="71"/>
+      <c r="C127" s="71"/>
       <c r="F127" s="13"/>
-      <c r="H127" s="71" t="s">
+      <c r="H127" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="I127" s="71"/>
-      <c r="J127" s="71"/>
-      <c r="K127" s="71"/>
-      <c r="L127" s="71"/>
-      <c r="M127" s="71"/>
+      <c r="I127" s="72"/>
+      <c r="J127" s="72"/>
+      <c r="K127" s="72"/>
+      <c r="L127" s="72"/>
+      <c r="M127" s="72"/>
       <c r="O127" s="73" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P127" s="73"/>
       <c r="Q127" s="73"/>
@@ -9410,8 +9411,8 @@
       <c r="T127" s="73"/>
     </row>
     <row r="128" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B128" s="70"/>
-      <c r="C128" s="70"/>
+      <c r="B128" s="71"/>
+      <c r="C128" s="71"/>
       <c r="F128" s="13"/>
       <c r="H128" s="16" t="s">
         <v>4</v>
@@ -9451,8 +9452,8 @@
       </c>
     </row>
     <row r="129" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B129" s="70"/>
-      <c r="C129" s="70"/>
+      <c r="B129" s="71"/>
+      <c r="C129" s="71"/>
       <c r="F129" s="13"/>
       <c r="H129" s="14">
         <f>H125+O125+O129</f>
@@ -9522,7 +9523,7 @@
     </row>
     <row r="131" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A131" s="74" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B131" s="74"/>
       <c r="C131" s="74"/>
@@ -9549,10 +9550,10 @@
       <c r="A132" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B132" s="79" t="s">
+      <c r="B132" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="C132" s="79"/>
+      <c r="C132" s="78"/>
       <c r="D132" s="55" t="s">
         <v>1</v>
       </c>
@@ -9590,18 +9591,18 @@
       <c r="A133" s="54">
         <v>21</v>
       </c>
-      <c r="B133" s="80" t="s">
-        <v>104</v>
-      </c>
-      <c r="C133" s="80"/>
+      <c r="B133" s="79" t="s">
+        <v>103</v>
+      </c>
+      <c r="C133" s="79"/>
       <c r="D133" s="50" t="s">
+        <v>105</v>
+      </c>
+      <c r="E133" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="E133" s="32" t="s">
+      <c r="F133" s="29" t="s">
         <v>107</v>
-      </c>
-      <c r="F133" s="29" t="s">
-        <v>108</v>
       </c>
       <c r="G133" s="54" t="s">
         <v>32</v>
@@ -9626,17 +9627,17 @@
         <v>22</v>
       </c>
       <c r="B134" s="81" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C134" s="81"/>
       <c r="D134" s="50" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E134" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="F134" s="29" t="s">
         <v>109</v>
-      </c>
-      <c r="F134" s="29" t="s">
-        <v>110</v>
       </c>
       <c r="G134" s="54" t="s">
         <v>32</v>
@@ -9657,8 +9658,8 @@
       <c r="Q134" s="52"/>
     </row>
     <row r="135" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B135" s="70"/>
-      <c r="C135" s="70"/>
+      <c r="B135" s="71"/>
+      <c r="C135" s="71"/>
       <c r="F135" s="13"/>
       <c r="H135" s="52"/>
       <c r="J135" s="52"/>
@@ -9667,8 +9668,8 @@
       <c r="Q135" s="52"/>
     </row>
     <row r="136" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B136" s="70"/>
-      <c r="C136" s="70"/>
+      <c r="B136" s="71"/>
+      <c r="C136" s="71"/>
       <c r="F136" s="13"/>
       <c r="H136" s="73" t="s">
         <v>19</v>
@@ -9679,7 +9680,7 @@
       <c r="L136" s="73"/>
       <c r="M136" s="73"/>
       <c r="O136" s="73" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P136" s="73"/>
       <c r="Q136" s="73"/>
@@ -9688,8 +9689,8 @@
       <c r="T136" s="73"/>
     </row>
     <row r="137" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B137" s="70"/>
-      <c r="C137" s="70"/>
+      <c r="B137" s="71"/>
+      <c r="C137" s="71"/>
       <c r="F137" s="13"/>
       <c r="H137" s="16" t="s">
         <v>4</v>
@@ -9729,8 +9730,8 @@
       </c>
     </row>
     <row r="138" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B138" s="70"/>
-      <c r="C138" s="70"/>
+      <c r="B138" s="71"/>
+      <c r="C138" s="71"/>
       <c r="F138" s="13"/>
       <c r="H138" s="14">
         <f>COUNTIF(H133:H134,"O")</f>
@@ -9782,8 +9783,8 @@
       </c>
     </row>
     <row r="139" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B139" s="70"/>
-      <c r="C139" s="70"/>
+      <c r="B139" s="71"/>
+      <c r="C139" s="71"/>
       <c r="F139" s="13"/>
       <c r="H139" s="52"/>
       <c r="J139" s="52"/>
@@ -9792,19 +9793,19 @@
       <c r="Q139"/>
     </row>
     <row r="140" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B140" s="70"/>
-      <c r="C140" s="70"/>
+      <c r="B140" s="71"/>
+      <c r="C140" s="71"/>
       <c r="F140" s="13"/>
-      <c r="H140" s="71" t="s">
+      <c r="H140" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="I140" s="71"/>
-      <c r="J140" s="71"/>
-      <c r="K140" s="71"/>
-      <c r="L140" s="71"/>
-      <c r="M140" s="71"/>
+      <c r="I140" s="72"/>
+      <c r="J140" s="72"/>
+      <c r="K140" s="72"/>
+      <c r="L140" s="72"/>
+      <c r="M140" s="72"/>
       <c r="O140" s="73" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P140" s="73"/>
       <c r="Q140" s="73"/>
@@ -9813,8 +9814,8 @@
       <c r="T140" s="73"/>
     </row>
     <row r="141" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B141" s="70"/>
-      <c r="C141" s="70"/>
+      <c r="B141" s="71"/>
+      <c r="C141" s="71"/>
       <c r="F141" s="13"/>
       <c r="H141" s="16" t="s">
         <v>4</v>
@@ -9854,8 +9855,8 @@
       </c>
     </row>
     <row r="142" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B142" s="70"/>
-      <c r="C142" s="70"/>
+      <c r="B142" s="71"/>
+      <c r="C142" s="71"/>
       <c r="F142" s="13"/>
       <c r="H142" s="14">
         <f>H138+O138+O142</f>
@@ -9908,8 +9909,8 @@
     </row>
     <row r="143" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A143" s="40"/>
-      <c r="B143" s="72"/>
-      <c r="C143" s="72"/>
+      <c r="B143" s="80"/>
+      <c r="C143" s="80"/>
       <c r="D143" s="40"/>
       <c r="E143" s="40"/>
       <c r="F143" s="41"/>
@@ -9926,7 +9927,7 @@
     </row>
     <row r="144" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A144" s="74" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B144" s="74"/>
       <c r="C144" s="74"/>
@@ -9953,10 +9954,10 @@
       <c r="A145" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B145" s="79" t="s">
+      <c r="B145" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="C145" s="79"/>
+      <c r="C145" s="78"/>
       <c r="D145" s="55" t="s">
         <v>1</v>
       </c>
@@ -9994,18 +9995,18 @@
       <c r="A146" s="54">
         <v>23</v>
       </c>
-      <c r="B146" s="80" t="s">
-        <v>112</v>
-      </c>
-      <c r="C146" s="80"/>
+      <c r="B146" s="79" t="s">
+        <v>111</v>
+      </c>
+      <c r="C146" s="79"/>
       <c r="D146" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E146" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="F146" s="29" t="s">
         <v>116</v>
-      </c>
-      <c r="F146" s="29" t="s">
-        <v>117</v>
       </c>
       <c r="G146" s="54" t="s">
         <v>32</v>
@@ -10030,17 +10031,17 @@
         <v>24</v>
       </c>
       <c r="B147" s="81" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C147" s="81"/>
       <c r="D147" s="50" t="s">
+        <v>117</v>
+      </c>
+      <c r="E147" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="F147" s="29" t="s">
         <v>118</v>
-      </c>
-      <c r="E147" s="32" t="s">
-        <v>116</v>
-      </c>
-      <c r="F147" s="29" t="s">
-        <v>119</v>
       </c>
       <c r="G147" s="54" t="s">
         <v>32</v>
@@ -10061,8 +10062,8 @@
       <c r="Q147" s="52"/>
     </row>
     <row r="148" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B148" s="70"/>
-      <c r="C148" s="70"/>
+      <c r="B148" s="71"/>
+      <c r="C148" s="71"/>
       <c r="F148" s="13"/>
       <c r="H148" s="52"/>
       <c r="J148" s="52"/>
@@ -10071,8 +10072,8 @@
       <c r="Q148" s="52"/>
     </row>
     <row r="149" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B149" s="70"/>
-      <c r="C149" s="70"/>
+      <c r="B149" s="71"/>
+      <c r="C149" s="71"/>
       <c r="F149" s="13"/>
       <c r="H149" s="73" t="s">
         <v>19</v>
@@ -10083,7 +10084,7 @@
       <c r="L149" s="73"/>
       <c r="M149" s="73"/>
       <c r="O149" s="73" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P149" s="73"/>
       <c r="Q149" s="73"/>
@@ -10092,8 +10093,8 @@
       <c r="T149" s="73"/>
     </row>
     <row r="150" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B150" s="70"/>
-      <c r="C150" s="70"/>
+      <c r="B150" s="71"/>
+      <c r="C150" s="71"/>
       <c r="F150" s="13"/>
       <c r="H150" s="16" t="s">
         <v>4</v>
@@ -10133,8 +10134,8 @@
       </c>
     </row>
     <row r="151" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B151" s="70"/>
-      <c r="C151" s="70"/>
+      <c r="B151" s="71"/>
+      <c r="C151" s="71"/>
       <c r="F151" s="13"/>
       <c r="H151" s="14">
         <f>COUNTIF(H146:H147,"O")</f>
@@ -10186,8 +10187,8 @@
       </c>
     </row>
     <row r="152" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B152" s="70"/>
-      <c r="C152" s="70"/>
+      <c r="B152" s="71"/>
+      <c r="C152" s="71"/>
       <c r="F152" s="13"/>
       <c r="H152" s="52"/>
       <c r="J152" s="52"/>
@@ -10196,19 +10197,19 @@
       <c r="Q152"/>
     </row>
     <row r="153" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B153" s="70"/>
-      <c r="C153" s="70"/>
+      <c r="B153" s="71"/>
+      <c r="C153" s="71"/>
       <c r="F153" s="13"/>
-      <c r="H153" s="71" t="s">
+      <c r="H153" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="I153" s="71"/>
-      <c r="J153" s="71"/>
-      <c r="K153" s="71"/>
-      <c r="L153" s="71"/>
-      <c r="M153" s="71"/>
+      <c r="I153" s="72"/>
+      <c r="J153" s="72"/>
+      <c r="K153" s="72"/>
+      <c r="L153" s="72"/>
+      <c r="M153" s="72"/>
       <c r="O153" s="73" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P153" s="73"/>
       <c r="Q153" s="73"/>
@@ -10217,8 +10218,8 @@
       <c r="T153" s="73"/>
     </row>
     <row r="154" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B154" s="70"/>
-      <c r="C154" s="70"/>
+      <c r="B154" s="71"/>
+      <c r="C154" s="71"/>
       <c r="F154" s="13"/>
       <c r="H154" s="16" t="s">
         <v>4</v>
@@ -10258,8 +10259,8 @@
       </c>
     </row>
     <row r="155" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B155" s="70"/>
-      <c r="C155" s="70"/>
+      <c r="B155" s="71"/>
+      <c r="C155" s="71"/>
       <c r="F155" s="13"/>
       <c r="H155" s="14">
         <f>H151+O151+O155</f>
@@ -10312,8 +10313,8 @@
     </row>
     <row r="156" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A156" s="40"/>
-      <c r="B156" s="72"/>
-      <c r="C156" s="72"/>
+      <c r="B156" s="80"/>
+      <c r="C156" s="80"/>
       <c r="D156" s="40"/>
       <c r="E156" s="40"/>
       <c r="F156" s="41"/>
@@ -10330,7 +10331,7 @@
     </row>
     <row r="157" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A157" s="74" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B157" s="74"/>
       <c r="C157" s="74"/>
@@ -10357,10 +10358,10 @@
       <c r="A158" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B158" s="79" t="s">
+      <c r="B158" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="C158" s="79"/>
+      <c r="C158" s="78"/>
       <c r="D158" s="55" t="s">
         <v>1</v>
       </c>
@@ -10398,18 +10399,18 @@
       <c r="A159" s="54">
         <v>25</v>
       </c>
-      <c r="B159" s="80" t="s">
-        <v>114</v>
-      </c>
-      <c r="C159" s="80"/>
+      <c r="B159" s="79" t="s">
+        <v>113</v>
+      </c>
+      <c r="C159" s="79"/>
       <c r="D159" s="50" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E159" s="32" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F159" s="29" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G159" s="54" t="s">
         <v>32</v>
@@ -10430,8 +10431,8 @@
       <c r="Q159" s="52"/>
     </row>
     <row r="160" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B160" s="70"/>
-      <c r="C160" s="70"/>
+      <c r="B160" s="71"/>
+      <c r="C160" s="71"/>
       <c r="F160" s="13"/>
       <c r="H160" s="52"/>
       <c r="J160" s="52"/>
@@ -10440,8 +10441,8 @@
       <c r="Q160" s="52"/>
     </row>
     <row r="161" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B161" s="70"/>
-      <c r="C161" s="70"/>
+      <c r="B161" s="71"/>
+      <c r="C161" s="71"/>
       <c r="F161" s="13"/>
       <c r="H161" s="73" t="s">
         <v>19</v>
@@ -10452,7 +10453,7 @@
       <c r="L161" s="73"/>
       <c r="M161" s="73"/>
       <c r="O161" s="73" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P161" s="73"/>
       <c r="Q161" s="73"/>
@@ -10461,10 +10462,10 @@
       <c r="T161" s="73"/>
     </row>
     <row r="162" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B162" s="70"/>
-      <c r="C162" s="70"/>
+      <c r="B162" s="71"/>
+      <c r="C162" s="71"/>
       <c r="E162" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F162" s="13"/>
       <c r="H162" s="16" t="s">
@@ -10505,8 +10506,8 @@
       </c>
     </row>
     <row r="163" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B163" s="70"/>
-      <c r="C163" s="70"/>
+      <c r="B163" s="71"/>
+      <c r="C163" s="71"/>
       <c r="F163" s="13"/>
       <c r="H163" s="14">
         <f>COUNTIF(H159:H159,"O")</f>
@@ -10558,8 +10559,8 @@
       </c>
     </row>
     <row r="164" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B164" s="70"/>
-      <c r="C164" s="70"/>
+      <c r="B164" s="71"/>
+      <c r="C164" s="71"/>
       <c r="F164" s="13"/>
       <c r="H164" s="52"/>
       <c r="J164" s="52"/>
@@ -10568,19 +10569,19 @@
       <c r="Q164"/>
     </row>
     <row r="165" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B165" s="70"/>
-      <c r="C165" s="70"/>
+      <c r="B165" s="71"/>
+      <c r="C165" s="71"/>
       <c r="F165" s="13"/>
-      <c r="H165" s="71" t="s">
+      <c r="H165" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="I165" s="71"/>
-      <c r="J165" s="71"/>
-      <c r="K165" s="71"/>
-      <c r="L165" s="71"/>
-      <c r="M165" s="71"/>
+      <c r="I165" s="72"/>
+      <c r="J165" s="72"/>
+      <c r="K165" s="72"/>
+      <c r="L165" s="72"/>
+      <c r="M165" s="72"/>
       <c r="O165" s="73" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P165" s="73"/>
       <c r="Q165" s="73"/>
@@ -10589,8 +10590,8 @@
       <c r="T165" s="73"/>
     </row>
     <row r="166" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B166" s="70"/>
-      <c r="C166" s="70"/>
+      <c r="B166" s="71"/>
+      <c r="C166" s="71"/>
       <c r="F166" s="13"/>
       <c r="H166" s="16" t="s">
         <v>4</v>
@@ -10630,8 +10631,8 @@
       </c>
     </row>
     <row r="167" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B167" s="70"/>
-      <c r="C167" s="70"/>
+      <c r="B167" s="71"/>
+      <c r="C167" s="71"/>
       <c r="F167" s="13"/>
       <c r="H167" s="14">
         <f>H163+O163+O167</f>
@@ -10684,8 +10685,8 @@
     </row>
     <row r="168" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A168" s="40"/>
-      <c r="B168" s="72"/>
-      <c r="C168" s="72"/>
+      <c r="B168" s="80"/>
+      <c r="C168" s="80"/>
       <c r="D168" s="40"/>
       <c r="E168" s="40"/>
       <c r="F168" s="41"/>
@@ -10702,7 +10703,7 @@
     </row>
     <row r="169" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A169" s="74" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B169" s="74"/>
       <c r="C169" s="74"/>
@@ -10729,10 +10730,10 @@
       <c r="A170" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="B170" s="79" t="s">
+      <c r="B170" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="C170" s="79"/>
+      <c r="C170" s="78"/>
       <c r="D170" s="60" t="s">
         <v>1</v>
       </c>
@@ -10770,18 +10771,18 @@
       <c r="A171" s="58">
         <v>26</v>
       </c>
-      <c r="B171" s="80" t="s">
-        <v>131</v>
-      </c>
-      <c r="C171" s="80"/>
+      <c r="B171" s="79" t="s">
+        <v>130</v>
+      </c>
+      <c r="C171" s="79"/>
       <c r="D171" s="50" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E171" s="32" t="s">
+        <v>152</v>
+      </c>
+      <c r="F171" s="29" t="s">
         <v>153</v>
-      </c>
-      <c r="F171" s="29" t="s">
-        <v>154</v>
       </c>
       <c r="G171" s="58" t="s">
         <v>32</v>
@@ -10802,8 +10803,8 @@
       <c r="Q171" s="56"/>
     </row>
     <row r="172" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B172" s="70"/>
-      <c r="C172" s="70"/>
+      <c r="B172" s="71"/>
+      <c r="C172" s="71"/>
       <c r="F172" s="13"/>
       <c r="H172" s="56"/>
       <c r="J172" s="56"/>
@@ -10812,8 +10813,8 @@
       <c r="Q172" s="56"/>
     </row>
     <row r="173" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B173" s="70"/>
-      <c r="C173" s="70"/>
+      <c r="B173" s="71"/>
+      <c r="C173" s="71"/>
       <c r="F173" s="13"/>
       <c r="H173" s="73" t="s">
         <v>19</v>
@@ -10824,7 +10825,7 @@
       <c r="L173" s="73"/>
       <c r="M173" s="73"/>
       <c r="O173" s="73" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P173" s="73"/>
       <c r="Q173" s="73"/>
@@ -10833,8 +10834,8 @@
       <c r="T173" s="73"/>
     </row>
     <row r="174" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B174" s="70"/>
-      <c r="C174" s="70"/>
+      <c r="B174" s="71"/>
+      <c r="C174" s="71"/>
       <c r="F174" s="13"/>
       <c r="H174" s="16" t="s">
         <v>4</v>
@@ -10874,8 +10875,8 @@
       </c>
     </row>
     <row r="175" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B175" s="70"/>
-      <c r="C175" s="70"/>
+      <c r="B175" s="71"/>
+      <c r="C175" s="71"/>
       <c r="F175" s="13"/>
       <c r="H175" s="14">
         <f>COUNTIF(H171:H171,"O")</f>
@@ -10927,8 +10928,8 @@
       </c>
     </row>
     <row r="176" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B176" s="70"/>
-      <c r="C176" s="70"/>
+      <c r="B176" s="71"/>
+      <c r="C176" s="71"/>
       <c r="F176" s="13"/>
       <c r="H176" s="56"/>
       <c r="J176" s="56"/>
@@ -10937,19 +10938,19 @@
       <c r="Q176"/>
     </row>
     <row r="177" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B177" s="70"/>
-      <c r="C177" s="70"/>
+      <c r="B177" s="71"/>
+      <c r="C177" s="71"/>
       <c r="F177" s="13"/>
-      <c r="H177" s="71" t="s">
+      <c r="H177" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="I177" s="71"/>
-      <c r="J177" s="71"/>
-      <c r="K177" s="71"/>
-      <c r="L177" s="71"/>
-      <c r="M177" s="71"/>
+      <c r="I177" s="72"/>
+      <c r="J177" s="72"/>
+      <c r="K177" s="72"/>
+      <c r="L177" s="72"/>
+      <c r="M177" s="72"/>
       <c r="O177" s="73" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P177" s="73"/>
       <c r="Q177" s="73"/>
@@ -10958,8 +10959,8 @@
       <c r="T177" s="73"/>
     </row>
     <row r="178" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B178" s="70"/>
-      <c r="C178" s="70"/>
+      <c r="B178" s="71"/>
+      <c r="C178" s="71"/>
       <c r="F178" s="13"/>
       <c r="H178" s="16" t="s">
         <v>4</v>
@@ -10999,8 +11000,8 @@
       </c>
     </row>
     <row r="179" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B179" s="70"/>
-      <c r="C179" s="70"/>
+      <c r="B179" s="71"/>
+      <c r="C179" s="71"/>
       <c r="F179" s="13"/>
       <c r="H179" s="14">
         <f>H175+O175+O179</f>
@@ -11053,8 +11054,8 @@
     </row>
     <row r="180" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A180" s="40"/>
-      <c r="B180" s="72"/>
-      <c r="C180" s="72"/>
+      <c r="B180" s="80"/>
+      <c r="C180" s="80"/>
       <c r="D180" s="40"/>
       <c r="E180" s="40"/>
       <c r="F180" s="41"/>
@@ -11071,7 +11072,7 @@
     </row>
     <row r="181" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A181" s="74" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B181" s="74"/>
       <c r="C181" s="74"/>
@@ -11098,10 +11099,10 @@
       <c r="A182" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B182" s="79" t="s">
+      <c r="B182" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="C182" s="79"/>
+      <c r="C182" s="78"/>
       <c r="D182" s="38" t="s">
         <v>1</v>
       </c>
@@ -11139,18 +11140,18 @@
       <c r="A183" s="39">
         <v>27</v>
       </c>
-      <c r="B183" s="80" t="s">
+      <c r="B183" s="79" t="s">
+        <v>63</v>
+      </c>
+      <c r="C183" s="79"/>
+      <c r="D183" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="E183" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="C183" s="80"/>
-      <c r="D183" s="34" t="s">
-        <v>64</v>
-      </c>
-      <c r="E183" s="32" t="s">
+      <c r="F183" s="29" t="s">
         <v>65</v>
-      </c>
-      <c r="F183" s="29" t="s">
-        <v>66</v>
       </c>
       <c r="G183" s="39" t="s">
         <v>32</v>
@@ -11175,17 +11176,17 @@
         <v>28</v>
       </c>
       <c r="B184" s="81" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C184" s="81"/>
       <c r="D184" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="E184" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="F184" s="29" t="s">
         <v>68</v>
-      </c>
-      <c r="E184" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="F184" s="29" t="s">
-        <v>69</v>
       </c>
       <c r="G184" s="39" t="s">
         <v>32</v>
@@ -11209,18 +11210,18 @@
       <c r="A185" s="68">
         <v>29</v>
       </c>
-      <c r="B185" s="78" t="s">
-        <v>64</v>
-      </c>
-      <c r="C185" s="78"/>
+      <c r="B185" s="70" t="s">
+        <v>63</v>
+      </c>
+      <c r="C185" s="70"/>
       <c r="D185" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E185" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="F185" s="29" t="s">
         <v>70</v>
-      </c>
-      <c r="F185" s="29" t="s">
-        <v>71</v>
       </c>
       <c r="G185" s="39" t="s">
         <v>32</v>
@@ -11244,18 +11245,18 @@
       <c r="A186" s="68">
         <v>30</v>
       </c>
-      <c r="B186" s="78" t="s">
-        <v>64</v>
-      </c>
-      <c r="C186" s="78"/>
+      <c r="B186" s="70" t="s">
+        <v>63</v>
+      </c>
+      <c r="C186" s="70"/>
       <c r="D186" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E186" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F186" s="29" t="s">
         <v>72</v>
-      </c>
-      <c r="F186" s="29" t="s">
-        <v>73</v>
       </c>
       <c r="G186" s="44" t="s">
         <v>32</v>
@@ -11279,18 +11280,18 @@
       <c r="A187" s="68">
         <v>31</v>
       </c>
-      <c r="B187" s="78" t="s">
-        <v>64</v>
-      </c>
-      <c r="C187" s="78"/>
+      <c r="B187" s="70" t="s">
+        <v>63</v>
+      </c>
+      <c r="C187" s="70"/>
       <c r="D187" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E187" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="F187" s="29" t="s">
         <v>74</v>
-      </c>
-      <c r="F187" s="29" t="s">
-        <v>75</v>
       </c>
       <c r="G187" s="44" t="s">
         <v>32</v>
@@ -11314,18 +11315,18 @@
       <c r="A188" s="68">
         <v>32</v>
       </c>
-      <c r="B188" s="78" t="s">
-        <v>64</v>
-      </c>
-      <c r="C188" s="78"/>
+      <c r="B188" s="70" t="s">
+        <v>63</v>
+      </c>
+      <c r="C188" s="70"/>
       <c r="D188" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E188" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="F188" s="29" t="s">
         <v>76</v>
-      </c>
-      <c r="F188" s="29" t="s">
-        <v>77</v>
       </c>
       <c r="G188" s="44" t="s">
         <v>32</v>
@@ -11349,18 +11350,18 @@
       <c r="A189" s="68">
         <v>33</v>
       </c>
-      <c r="B189" s="78" t="s">
-        <v>64</v>
-      </c>
-      <c r="C189" s="78"/>
+      <c r="B189" s="70" t="s">
+        <v>63</v>
+      </c>
+      <c r="C189" s="70"/>
       <c r="D189" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="E189" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="E189" s="32" t="s">
+      <c r="F189" s="29" t="s">
         <v>79</v>
-      </c>
-      <c r="F189" s="29" t="s">
-        <v>80</v>
       </c>
       <c r="G189" s="44" t="s">
         <v>32</v>
@@ -11384,18 +11385,18 @@
       <c r="A190" s="68">
         <v>34</v>
       </c>
-      <c r="B190" s="78" t="s">
-        <v>64</v>
-      </c>
-      <c r="C190" s="78"/>
+      <c r="B190" s="70" t="s">
+        <v>63</v>
+      </c>
+      <c r="C190" s="70"/>
       <c r="D190" s="34" t="s">
+        <v>98</v>
+      </c>
+      <c r="E190" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="E190" s="32" t="s">
+      <c r="F190" s="29" t="s">
         <v>100</v>
-      </c>
-      <c r="F190" s="29" t="s">
-        <v>101</v>
       </c>
       <c r="G190" s="44" t="s">
         <v>32</v>
@@ -11416,8 +11417,8 @@
       <c r="Q190" s="43"/>
     </row>
     <row r="191" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B191" s="70"/>
-      <c r="C191" s="70"/>
+      <c r="B191" s="71"/>
+      <c r="C191" s="71"/>
       <c r="F191" s="13"/>
       <c r="H191" s="43"/>
       <c r="J191" s="43"/>
@@ -11426,8 +11427,8 @@
       <c r="Q191" s="43"/>
     </row>
     <row r="192" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B192" s="70"/>
-      <c r="C192" s="70"/>
+      <c r="B192" s="71"/>
+      <c r="C192" s="71"/>
       <c r="F192" s="13"/>
       <c r="H192" s="73" t="s">
         <v>19</v>
@@ -11438,7 +11439,7 @@
       <c r="L192" s="73"/>
       <c r="M192" s="73"/>
       <c r="O192" s="73" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P192" s="73"/>
       <c r="Q192" s="73"/>
@@ -11447,8 +11448,8 @@
       <c r="T192" s="73"/>
     </row>
     <row r="193" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B193" s="70"/>
-      <c r="C193" s="70"/>
+      <c r="B193" s="71"/>
+      <c r="C193" s="71"/>
       <c r="F193" s="13"/>
       <c r="H193" s="16" t="s">
         <v>4</v>
@@ -11488,8 +11489,8 @@
       </c>
     </row>
     <row r="194" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B194" s="70"/>
-      <c r="C194" s="70"/>
+      <c r="B194" s="71"/>
+      <c r="C194" s="71"/>
       <c r="F194" s="13"/>
       <c r="H194" s="14">
         <f>COUNTIF(H183:H190,"O")</f>
@@ -11541,8 +11542,8 @@
       </c>
     </row>
     <row r="195" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B195" s="70"/>
-      <c r="C195" s="70"/>
+      <c r="B195" s="71"/>
+      <c r="C195" s="71"/>
       <c r="F195" s="13"/>
       <c r="H195" s="43"/>
       <c r="J195" s="43"/>
@@ -11551,19 +11552,19 @@
       <c r="Q195"/>
     </row>
     <row r="196" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B196" s="70"/>
-      <c r="C196" s="70"/>
+      <c r="B196" s="71"/>
+      <c r="C196" s="71"/>
       <c r="F196" s="13"/>
-      <c r="H196" s="71" t="s">
+      <c r="H196" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="I196" s="71"/>
-      <c r="J196" s="71"/>
-      <c r="K196" s="71"/>
-      <c r="L196" s="71"/>
-      <c r="M196" s="71"/>
+      <c r="I196" s="72"/>
+      <c r="J196" s="72"/>
+      <c r="K196" s="72"/>
+      <c r="L196" s="72"/>
+      <c r="M196" s="72"/>
       <c r="O196" s="73" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P196" s="73"/>
       <c r="Q196" s="73"/>
@@ -11572,8 +11573,8 @@
       <c r="T196" s="73"/>
     </row>
     <row r="197" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B197" s="70"/>
-      <c r="C197" s="70"/>
+      <c r="B197" s="71"/>
+      <c r="C197" s="71"/>
       <c r="F197" s="13"/>
       <c r="H197" s="16" t="s">
         <v>4</v>
@@ -11613,8 +11614,8 @@
       </c>
     </row>
     <row r="198" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B198" s="70"/>
-      <c r="C198" s="70"/>
+      <c r="B198" s="71"/>
+      <c r="C198" s="71"/>
       <c r="F198" s="13"/>
       <c r="H198" s="14">
         <f>H194+O194+O198</f>
@@ -11667,8 +11668,8 @@
     </row>
     <row r="199" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A199" s="40"/>
-      <c r="B199" s="72"/>
-      <c r="C199" s="72"/>
+      <c r="B199" s="80"/>
+      <c r="C199" s="80"/>
       <c r="D199" s="40"/>
       <c r="E199" s="40"/>
       <c r="F199" s="41"/>
@@ -11685,6 +11686,270 @@
     </row>
   </sheetData>
   <mergeCells count="288">
+    <mergeCell ref="B196:C196"/>
+    <mergeCell ref="H196:M196"/>
+    <mergeCell ref="B197:C197"/>
+    <mergeCell ref="B198:C198"/>
+    <mergeCell ref="B199:C199"/>
+    <mergeCell ref="B192:C192"/>
+    <mergeCell ref="H192:M192"/>
+    <mergeCell ref="B193:C193"/>
+    <mergeCell ref="B194:C194"/>
+    <mergeCell ref="B195:C195"/>
+    <mergeCell ref="B191:C191"/>
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="A181:G181"/>
+    <mergeCell ref="H181:I181"/>
+    <mergeCell ref="J181:K181"/>
+    <mergeCell ref="B186:C186"/>
+    <mergeCell ref="B187:C187"/>
+    <mergeCell ref="B188:C188"/>
+    <mergeCell ref="B189:C189"/>
+    <mergeCell ref="B190:C190"/>
+    <mergeCell ref="B114:C114"/>
+    <mergeCell ref="B115:C115"/>
+    <mergeCell ref="H115:M115"/>
+    <mergeCell ref="B116:C116"/>
+    <mergeCell ref="B117:C117"/>
+    <mergeCell ref="B143:C143"/>
+    <mergeCell ref="L181:M181"/>
+    <mergeCell ref="A106:G106"/>
+    <mergeCell ref="H106:I106"/>
+    <mergeCell ref="A169:G169"/>
+    <mergeCell ref="H169:I169"/>
+    <mergeCell ref="J169:K169"/>
+    <mergeCell ref="L169:M169"/>
+    <mergeCell ref="B170:C170"/>
+    <mergeCell ref="B97:C97"/>
+    <mergeCell ref="B98:C98"/>
+    <mergeCell ref="H98:M98"/>
+    <mergeCell ref="B99:C99"/>
+    <mergeCell ref="B100:C100"/>
+    <mergeCell ref="B182:C182"/>
+    <mergeCell ref="B183:C183"/>
+    <mergeCell ref="B184:C184"/>
+    <mergeCell ref="B185:C185"/>
+    <mergeCell ref="B171:C171"/>
+    <mergeCell ref="B172:C172"/>
+    <mergeCell ref="B173:C173"/>
+    <mergeCell ref="H173:M173"/>
+    <mergeCell ref="B174:C174"/>
+    <mergeCell ref="B175:C175"/>
+    <mergeCell ref="B176:C176"/>
+    <mergeCell ref="B177:C177"/>
+    <mergeCell ref="H177:M177"/>
+    <mergeCell ref="B178:C178"/>
+    <mergeCell ref="B179:C179"/>
+    <mergeCell ref="B180:C180"/>
+    <mergeCell ref="B113:C113"/>
+    <mergeCell ref="J106:K106"/>
+    <mergeCell ref="L106:M106"/>
+    <mergeCell ref="L93:M93"/>
+    <mergeCell ref="B94:C94"/>
+    <mergeCell ref="B95:C95"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="B91:C91"/>
+    <mergeCell ref="B92:C92"/>
+    <mergeCell ref="A93:G93"/>
+    <mergeCell ref="H93:I93"/>
+    <mergeCell ref="J93:K93"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="B108:C108"/>
+    <mergeCell ref="B109:C109"/>
+    <mergeCell ref="B110:C110"/>
+    <mergeCell ref="B111:C111"/>
+    <mergeCell ref="H111:M111"/>
+    <mergeCell ref="B112:C112"/>
+    <mergeCell ref="B101:C101"/>
+    <mergeCell ref="B102:C102"/>
+    <mergeCell ref="H102:M102"/>
+    <mergeCell ref="B103:C103"/>
+    <mergeCell ref="B104:C104"/>
+    <mergeCell ref="B87:C87"/>
+    <mergeCell ref="B88:C88"/>
+    <mergeCell ref="B89:C89"/>
+    <mergeCell ref="H89:M89"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="H85:M85"/>
+    <mergeCell ref="B86:C86"/>
+    <mergeCell ref="J81:K81"/>
+    <mergeCell ref="L81:M81"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="A81:G81"/>
+    <mergeCell ref="H81:I81"/>
+    <mergeCell ref="H73:M73"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="H77:M77"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="A69:G69"/>
+    <mergeCell ref="H69:I69"/>
+    <mergeCell ref="J69:K69"/>
+    <mergeCell ref="L69:M69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="H33:M33"/>
+    <mergeCell ref="H37:M37"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="L41:M41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H20:M20"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="H16:M16"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="A41:G41"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="H48:M48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="H52:M52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="H65:M65"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="A56:G56"/>
+    <mergeCell ref="H56:I56"/>
+    <mergeCell ref="J56:K56"/>
+    <mergeCell ref="L56:M56"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="H61:M61"/>
+    <mergeCell ref="O16:T16"/>
+    <mergeCell ref="O20:T20"/>
+    <mergeCell ref="O33:T33"/>
+    <mergeCell ref="O37:T37"/>
+    <mergeCell ref="O61:T61"/>
+    <mergeCell ref="O65:T65"/>
+    <mergeCell ref="O73:T73"/>
+    <mergeCell ref="O77:T77"/>
+    <mergeCell ref="O85:T85"/>
+    <mergeCell ref="O192:T192"/>
+    <mergeCell ref="O196:T196"/>
+    <mergeCell ref="O48:T48"/>
+    <mergeCell ref="O52:T52"/>
+    <mergeCell ref="O111:T111"/>
+    <mergeCell ref="O115:T115"/>
+    <mergeCell ref="O136:T136"/>
+    <mergeCell ref="O173:T173"/>
+    <mergeCell ref="O177:T177"/>
+    <mergeCell ref="O123:T123"/>
+    <mergeCell ref="B137:C137"/>
+    <mergeCell ref="B138:C138"/>
+    <mergeCell ref="B139:C139"/>
+    <mergeCell ref="B140:C140"/>
+    <mergeCell ref="H140:M140"/>
+    <mergeCell ref="O140:T140"/>
+    <mergeCell ref="B141:C141"/>
+    <mergeCell ref="B142:C142"/>
+    <mergeCell ref="A131:G131"/>
+    <mergeCell ref="H131:I131"/>
+    <mergeCell ref="J131:K131"/>
+    <mergeCell ref="L131:M131"/>
+    <mergeCell ref="B132:C132"/>
+    <mergeCell ref="B133:C133"/>
+    <mergeCell ref="B134:C134"/>
+    <mergeCell ref="B135:C135"/>
+    <mergeCell ref="B136:C136"/>
+    <mergeCell ref="H136:M136"/>
+    <mergeCell ref="A144:G144"/>
+    <mergeCell ref="H144:I144"/>
+    <mergeCell ref="J144:K144"/>
+    <mergeCell ref="L144:M144"/>
+    <mergeCell ref="H149:M149"/>
+    <mergeCell ref="O149:T149"/>
+    <mergeCell ref="H153:M153"/>
+    <mergeCell ref="O153:T153"/>
+    <mergeCell ref="B145:C145"/>
+    <mergeCell ref="B146:C146"/>
+    <mergeCell ref="B147:C147"/>
+    <mergeCell ref="B148:C148"/>
+    <mergeCell ref="B149:C149"/>
+    <mergeCell ref="B150:C150"/>
+    <mergeCell ref="B155:C155"/>
+    <mergeCell ref="B156:C156"/>
+    <mergeCell ref="A157:G157"/>
+    <mergeCell ref="H157:I157"/>
+    <mergeCell ref="J157:K157"/>
+    <mergeCell ref="L157:M157"/>
+    <mergeCell ref="B158:C158"/>
+    <mergeCell ref="B159:C159"/>
+    <mergeCell ref="B151:C151"/>
+    <mergeCell ref="B152:C152"/>
+    <mergeCell ref="B153:C153"/>
+    <mergeCell ref="B154:C154"/>
+    <mergeCell ref="B166:C166"/>
+    <mergeCell ref="B167:C167"/>
+    <mergeCell ref="B168:C168"/>
+    <mergeCell ref="B160:C160"/>
+    <mergeCell ref="B161:C161"/>
+    <mergeCell ref="H161:M161"/>
+    <mergeCell ref="O161:T161"/>
+    <mergeCell ref="B162:C162"/>
+    <mergeCell ref="B163:C163"/>
+    <mergeCell ref="B164:C164"/>
+    <mergeCell ref="B165:C165"/>
+    <mergeCell ref="H165:M165"/>
+    <mergeCell ref="O165:T165"/>
     <mergeCell ref="B46:C46"/>
     <mergeCell ref="B124:C124"/>
     <mergeCell ref="B125:C125"/>
@@ -11709,270 +11974,6 @@
     <mergeCell ref="B55:C55"/>
     <mergeCell ref="B66:C66"/>
     <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B166:C166"/>
-    <mergeCell ref="B167:C167"/>
-    <mergeCell ref="B168:C168"/>
-    <mergeCell ref="B160:C160"/>
-    <mergeCell ref="B161:C161"/>
-    <mergeCell ref="H161:M161"/>
-    <mergeCell ref="O161:T161"/>
-    <mergeCell ref="B162:C162"/>
-    <mergeCell ref="B163:C163"/>
-    <mergeCell ref="B164:C164"/>
-    <mergeCell ref="B165:C165"/>
-    <mergeCell ref="H165:M165"/>
-    <mergeCell ref="O165:T165"/>
-    <mergeCell ref="B155:C155"/>
-    <mergeCell ref="B156:C156"/>
-    <mergeCell ref="A157:G157"/>
-    <mergeCell ref="H157:I157"/>
-    <mergeCell ref="J157:K157"/>
-    <mergeCell ref="L157:M157"/>
-    <mergeCell ref="B158:C158"/>
-    <mergeCell ref="B159:C159"/>
-    <mergeCell ref="B151:C151"/>
-    <mergeCell ref="B152:C152"/>
-    <mergeCell ref="B153:C153"/>
-    <mergeCell ref="B154:C154"/>
-    <mergeCell ref="A144:G144"/>
-    <mergeCell ref="H144:I144"/>
-    <mergeCell ref="J144:K144"/>
-    <mergeCell ref="L144:M144"/>
-    <mergeCell ref="H149:M149"/>
-    <mergeCell ref="O149:T149"/>
-    <mergeCell ref="H153:M153"/>
-    <mergeCell ref="O153:T153"/>
-    <mergeCell ref="B145:C145"/>
-    <mergeCell ref="B146:C146"/>
-    <mergeCell ref="B147:C147"/>
-    <mergeCell ref="B148:C148"/>
-    <mergeCell ref="B149:C149"/>
-    <mergeCell ref="B150:C150"/>
-    <mergeCell ref="B137:C137"/>
-    <mergeCell ref="B138:C138"/>
-    <mergeCell ref="B139:C139"/>
-    <mergeCell ref="B140:C140"/>
-    <mergeCell ref="H140:M140"/>
-    <mergeCell ref="O140:T140"/>
-    <mergeCell ref="B141:C141"/>
-    <mergeCell ref="B142:C142"/>
-    <mergeCell ref="A131:G131"/>
-    <mergeCell ref="H131:I131"/>
-    <mergeCell ref="J131:K131"/>
-    <mergeCell ref="L131:M131"/>
-    <mergeCell ref="B132:C132"/>
-    <mergeCell ref="B133:C133"/>
-    <mergeCell ref="B134:C134"/>
-    <mergeCell ref="B135:C135"/>
-    <mergeCell ref="B136:C136"/>
-    <mergeCell ref="H136:M136"/>
-    <mergeCell ref="O192:T192"/>
-    <mergeCell ref="O196:T196"/>
-    <mergeCell ref="O48:T48"/>
-    <mergeCell ref="O52:T52"/>
-    <mergeCell ref="O111:T111"/>
-    <mergeCell ref="O115:T115"/>
-    <mergeCell ref="O136:T136"/>
-    <mergeCell ref="O173:T173"/>
-    <mergeCell ref="O177:T177"/>
-    <mergeCell ref="O123:T123"/>
-    <mergeCell ref="O16:T16"/>
-    <mergeCell ref="O20:T20"/>
-    <mergeCell ref="O33:T33"/>
-    <mergeCell ref="O37:T37"/>
-    <mergeCell ref="O61:T61"/>
-    <mergeCell ref="O65:T65"/>
-    <mergeCell ref="O73:T73"/>
-    <mergeCell ref="O77:T77"/>
-    <mergeCell ref="O85:T85"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="H65:M65"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="A56:G56"/>
-    <mergeCell ref="H56:I56"/>
-    <mergeCell ref="J56:K56"/>
-    <mergeCell ref="L56:M56"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="H61:M61"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="H48:M48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="H52:M52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="A41:G41"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="A25:G25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="H16:M16"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="H20:M20"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="A10:G10"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="A69:G69"/>
-    <mergeCell ref="H69:I69"/>
-    <mergeCell ref="J69:K69"/>
-    <mergeCell ref="L69:M69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="H33:M33"/>
-    <mergeCell ref="H37:M37"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="J41:K41"/>
-    <mergeCell ref="L41:M41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="H73:M73"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="H77:M77"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="J81:K81"/>
-    <mergeCell ref="L81:M81"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="A81:G81"/>
-    <mergeCell ref="H81:I81"/>
-    <mergeCell ref="B87:C87"/>
-    <mergeCell ref="B88:C88"/>
-    <mergeCell ref="B89:C89"/>
-    <mergeCell ref="H89:M89"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="H85:M85"/>
-    <mergeCell ref="B86:C86"/>
-    <mergeCell ref="B107:C107"/>
-    <mergeCell ref="B108:C108"/>
-    <mergeCell ref="B109:C109"/>
-    <mergeCell ref="B110:C110"/>
-    <mergeCell ref="B111:C111"/>
-    <mergeCell ref="H111:M111"/>
-    <mergeCell ref="B112:C112"/>
-    <mergeCell ref="B101:C101"/>
-    <mergeCell ref="B102:C102"/>
-    <mergeCell ref="H102:M102"/>
-    <mergeCell ref="B103:C103"/>
-    <mergeCell ref="B104:C104"/>
-    <mergeCell ref="L93:M93"/>
-    <mergeCell ref="B94:C94"/>
-    <mergeCell ref="B95:C95"/>
-    <mergeCell ref="B96:C96"/>
-    <mergeCell ref="B91:C91"/>
-    <mergeCell ref="B92:C92"/>
-    <mergeCell ref="A93:G93"/>
-    <mergeCell ref="H93:I93"/>
-    <mergeCell ref="J93:K93"/>
-    <mergeCell ref="B97:C97"/>
-    <mergeCell ref="B98:C98"/>
-    <mergeCell ref="H98:M98"/>
-    <mergeCell ref="B99:C99"/>
-    <mergeCell ref="B100:C100"/>
-    <mergeCell ref="B182:C182"/>
-    <mergeCell ref="B183:C183"/>
-    <mergeCell ref="B184:C184"/>
-    <mergeCell ref="B185:C185"/>
-    <mergeCell ref="B171:C171"/>
-    <mergeCell ref="B172:C172"/>
-    <mergeCell ref="B173:C173"/>
-    <mergeCell ref="H173:M173"/>
-    <mergeCell ref="B174:C174"/>
-    <mergeCell ref="B175:C175"/>
-    <mergeCell ref="B176:C176"/>
-    <mergeCell ref="B177:C177"/>
-    <mergeCell ref="H177:M177"/>
-    <mergeCell ref="B178:C178"/>
-    <mergeCell ref="B179:C179"/>
-    <mergeCell ref="B180:C180"/>
-    <mergeCell ref="B113:C113"/>
-    <mergeCell ref="J106:K106"/>
-    <mergeCell ref="L106:M106"/>
-    <mergeCell ref="B191:C191"/>
-    <mergeCell ref="B105:C105"/>
-    <mergeCell ref="A181:G181"/>
-    <mergeCell ref="H181:I181"/>
-    <mergeCell ref="J181:K181"/>
-    <mergeCell ref="B186:C186"/>
-    <mergeCell ref="B187:C187"/>
-    <mergeCell ref="B188:C188"/>
-    <mergeCell ref="B189:C189"/>
-    <mergeCell ref="B190:C190"/>
-    <mergeCell ref="B114:C114"/>
-    <mergeCell ref="B115:C115"/>
-    <mergeCell ref="H115:M115"/>
-    <mergeCell ref="B116:C116"/>
-    <mergeCell ref="B117:C117"/>
-    <mergeCell ref="B143:C143"/>
-    <mergeCell ref="L181:M181"/>
-    <mergeCell ref="A106:G106"/>
-    <mergeCell ref="H106:I106"/>
-    <mergeCell ref="A169:G169"/>
-    <mergeCell ref="H169:I169"/>
-    <mergeCell ref="J169:K169"/>
-    <mergeCell ref="L169:M169"/>
-    <mergeCell ref="B170:C170"/>
-    <mergeCell ref="B196:C196"/>
-    <mergeCell ref="H196:M196"/>
-    <mergeCell ref="B197:C197"/>
-    <mergeCell ref="B198:C198"/>
-    <mergeCell ref="B199:C199"/>
-    <mergeCell ref="B192:C192"/>
-    <mergeCell ref="H192:M192"/>
-    <mergeCell ref="B193:C193"/>
-    <mergeCell ref="B194:C194"/>
-    <mergeCell ref="B195:C195"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:B9">
     <cfRule type="colorScale" priority="1143">

</xml_diff>